<commit_message>
Add knockout stage drawing
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A533FEE6-5101-4971-A44F-3A0E16B8F166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15315" windowHeight="7995"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -37,41 +43,6 @@
     <t>L8</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Georgia"/>
-        <family val="1"/>
-      </rPr>
-      <t>PrintYour</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Georgia"/>
-        <family val="1"/>
-      </rPr>
-      <t>Brackets</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Georgia"/>
-        <family val="1"/>
-      </rPr>
-      <t>.com</t>
-    </r>
-  </si>
-  <si>
     <t>Loser's Bracket</t>
   </si>
   <si>
@@ -85,17 +56,49 @@
   </si>
   <si>
     <t>L14 If First Loss</t>
+  </si>
+  <si>
+    <t>沙隆巴斯</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>金贝贝</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰乔</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿土伯</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>莎拉公主</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>钱夫人</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>忍太郎</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>宫本宝藏</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -120,30 +123,9 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="3" tint="-0.249977111117893"/>
-      <name val="Georgia"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="3" tint="-0.249977111117893"/>
-      <name val="Georgia"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="Georgia"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Cambria"/>
+      <name val="宋体"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -164,6 +146,27 @@
       <color theme="0"/>
       <name val="Book Antiqua"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -300,46 +303,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -351,23 +354,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -409,7 +424,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,9 +456,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -475,6 +508,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -650,27 +701,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="7" width="12.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="17.42578125" style="1"/>
+    <col min="1" max="1" width="2.75" style="1" customWidth="1"/>
+    <col min="2" max="7" width="12.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="17.375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="11.1" customHeight="1">
+    <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
       <c r="B1" s="24"/>
       <c r="C1" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="31"/>
@@ -679,9 +730,9 @@
       <c r="H1" s="31"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" ht="11.1" customHeight="1">
+    <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="31"/>
@@ -692,43 +743,48 @@
       <c r="H2" s="31"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="11.85" customHeight="1">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="32" t="s">
+        <v>12</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <v>1</v>
       </c>
       <c r="C7" s="7"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
-      <c r="B8" s="6"/>
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="33" t="s">
+        <v>13</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="22">
         <v>7</v>
       </c>
@@ -736,65 +792,73 @@
       <c r="E11" s="7"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="34" t="s">
+        <v>14</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8"/>
       <c r="C14" s="12"/>
       <c r="E14" s="8"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8">
         <v>2</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
-      <c r="B16" s="6"/>
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="35" t="s">
+        <v>15</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E17" s="8"/>
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="18" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="8">
         <v>11</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="19" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="20" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="32" t="s">
+        <v>16</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="21" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="E21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="22" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="E22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="23" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
         <v>3</v>
       </c>
@@ -802,34 +866,39 @@
       <c r="E23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
-      <c r="B24" s="6"/>
+    <row r="24" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="33" t="s">
+        <v>17</v>
+      </c>
       <c r="C24" s="8"/>
       <c r="E24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="25" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
       <c r="E25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="26" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="D26" s="15"/>
       <c r="E26" s="6"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="27" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="8">
         <v>8</v>
       </c>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="28" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="32" t="s">
+        <v>18</v>
+      </c>
       <c r="C28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="29" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="G29" s="8">
@@ -837,34 +906,36 @@
       </c>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="30" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="12"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="31" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8">
         <v>4</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1">
-      <c r="B32" s="6"/>
+    <row r="32" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="E32" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="33" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="16"/>
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="34" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="16"/>
@@ -872,9 +943,9 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="35" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="20" t="s">
@@ -885,19 +956,19 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="36" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="37" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D37" s="8"/>
       <c r="F37" s="17"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="38" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
       <c r="B38" s="26" t="s">
         <v>1</v>
@@ -907,7 +978,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="39" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
       <c r="E39" s="15"/>
@@ -915,7 +986,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="40" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="8"/>
       <c r="D40" s="8">
         <v>9</v>
@@ -925,7 +996,7 @@
       <c r="G40" s="12"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="41" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -935,7 +1006,7 @@
       <c r="H41" s="8"/>
       <c r="I41" s="15"/>
     </row>
-    <row r="42" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="42" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
       <c r="C42" s="8"/>
       <c r="D42" s="6"/>
@@ -945,7 +1016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="43" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="8">
         <v>5</v>
       </c>
@@ -954,20 +1025,20 @@
       <c r="F43" s="8"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="44" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="45" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="8"/>
       <c r="D45" s="18"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="46" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20"/>
       <c r="B46" s="26" t="s">
         <v>2</v>
@@ -977,23 +1048,23 @@
       <c r="F46" s="8"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="47" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E47" s="8"/>
       <c r="F47" s="12"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="48" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E48" s="4">
         <v>12</v>
       </c>
       <c r="F48" s="18"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="49" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F49" s="18"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="50" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20"/>
       <c r="B50" s="16" t="s">
         <v>0</v>
@@ -1001,24 +1072,24 @@
       <c r="E50" s="8"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="51" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E51" s="8"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="52" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D52" s="7"/>
       <c r="E52" s="19"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="53" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D53" s="8"/>
       <c r="E53" s="19"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="54" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20"/>
       <c r="B54" s="26" t="s">
         <v>3</v>
@@ -1027,60 +1098,58 @@
       <c r="E54" s="19"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="7"/>
       <c r="D55" s="8"/>
       <c r="E55" s="12"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="8"/>
       <c r="D56" s="8">
         <v>10</v>
       </c>
       <c r="H56" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I56" s="23"/>
     </row>
-    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20"/>
       <c r="C58" s="8"/>
       <c r="D58" s="12"/>
     </row>
-    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20"/>
       <c r="B62" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C62" s="6"/>
     </row>
-    <row r="63" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
-      <c r="C63" s="27" t="s">
-        <v>7</v>
-      </c>
+    <row r="63" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="27"/>
       <c r="D63" s="27"/>
       <c r="E63" s="27"/>
       <c r="F63" s="27"/>
       <c r="G63" s="27"/>
       <c r="H63" s="27"/>
     </row>
-    <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1">
+    <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="27"/>
       <c r="D64" s="27"/>
       <c r="E64" s="27"/>
@@ -1088,7 +1157,7 @@
       <c r="G64" s="27"/>
       <c r="H64" s="27"/>
     </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" ht="11.85" customHeight="1">
+    <row r="65" spans="1:8" s="2" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="27"/>
       <c r="D65" s="27"/>
       <c r="E65" s="27"/>
@@ -1096,7 +1165,7 @@
       <c r="G65" s="27"/>
       <c r="H65" s="27"/>
     </row>
-    <row r="66" spans="1:8" ht="11.85" customHeight="1">
+    <row r="66" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
       <c r="C66" s="27"/>
       <c r="D66" s="27"/>
@@ -1105,7 +1174,7 @@
       <c r="G66" s="27"/>
       <c r="H66" s="27"/>
     </row>
-    <row r="67" spans="1:8" ht="13.5" customHeight="1">
+    <row r="67" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="27"/>
       <c r="D67" s="27"/>
       <c r="E67" s="27"/>
@@ -1121,7 +1190,8 @@
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C1:H2"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the knockout draw and match table
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A533FEE6-5101-4971-A44F-3A0E16B8F166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3271224-71A6-41E4-8F97-379B3BBCA896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -87,6 +87,22 @@
   </si>
   <si>
     <t>宫本宝藏</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙隆巴斯  0</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>金贝贝   2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰乔  0</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿土伯  2</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -303,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -345,6 +361,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -360,10 +380,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -704,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -720,27 +737,27 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
       <c r="B1" s="24"/>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -748,8 +765,8 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="32" t="s">
-        <v>12</v>
+      <c r="B4" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -760,6 +777,9 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
+      <c r="C6" s="27" t="s">
+        <v>13</v>
+      </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -770,8 +790,8 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="33" t="s">
-        <v>13</v>
+      <c r="B8" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="8"/>
       <c r="F8" s="5"/>
@@ -793,8 +813,8 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="34" t="s">
-        <v>14</v>
+      <c r="B12" s="29" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="8"/>
       <c r="E12" s="8"/>
@@ -807,7 +827,9 @@
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8"/>
-      <c r="C14" s="12"/>
+      <c r="C14" s="36" t="s">
+        <v>15</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="11"/>
     </row>
@@ -819,8 +841,8 @@
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="35" t="s">
-        <v>15</v>
+      <c r="B16" s="30" t="s">
+        <v>23</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="11"/>
@@ -842,7 +864,7 @@
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="27" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="8"/>
@@ -867,7 +889,7 @@
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="8"/>
@@ -892,7 +914,7 @@
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="8"/>
@@ -920,7 +942,7 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="20" t="s">
@@ -936,18 +958,18 @@
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="16"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="28"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="20" t="s">
         <v>6</v>
       </c>
@@ -968,10 +990,13 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="26" t="s">
         <v>1</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>12</v>
       </c>
       <c r="D38" s="8"/>
       <c r="F38" s="17"/>
@@ -1038,12 +1063,14 @@
       <c r="F45" s="8"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="20"/>
       <c r="B46" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="6"/>
+      <c r="C46" s="28" t="s">
+        <v>14</v>
+      </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="H46" s="8"/>
@@ -1142,45 +1169,45 @@
       <c r="C62" s="6"/>
     </row>
     <row r="63" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
     </row>
     <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="31"/>
     </row>
     <row r="65" spans="1:8" s="2" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
     </row>
     <row r="66" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="31"/>
+      <c r="H66" s="31"/>
     </row>
     <row r="67" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update on draw.py and excel
Add drawing rules for olympic basketballs
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022A8160-DF2E-4447-A57E-10364640A757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB1193E-0E23-4327-84CE-7DCF4C603126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -92,10 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>约翰乔(2-3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>钱夫人(1-2)  1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,11 +132,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>忍太郎(2-2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Winner's Bracket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忍太郎(2-2)   0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰乔(2-3)   2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰乔(4-3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -362,13 +366,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,12 +385,6 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,6 +396,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,487 +749,489 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="12" customWidth="1"/>
-    <col min="2" max="7" width="12.25" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="12" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="17.375" style="12"/>
+    <col min="1" max="1" width="2.75" style="11" customWidth="1"/>
+    <col min="2" max="7" width="12.25" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="17.375" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" s="14" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17"/>
-      <c r="F5" s="16"/>
+      <c r="B5" s="15"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="18"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="16"/>
+        <v>23</v>
+      </c>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="F7" s="16"/>
+      <c r="C7" s="15"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="F8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="18"/>
-      <c r="F9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="18"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="19">
+      <c r="C11" s="17">
         <v>7</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="C12" s="16"/>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="21"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="21"/>
+        <v>24</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="18">
+      <c r="B15" s="16">
         <v>2</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="21"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="21"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="18"/>
-      <c r="F17" s="22"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="18">
+      <c r="E18" s="16">
         <v>11</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="17"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="E19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="E20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
-      <c r="E21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="B21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="G22" s="18"/>
+        <v>27</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="18">
+      <c r="B23" s="16">
         <v>3</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="E23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="21"/>
+      <c r="E23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="18"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="G26" s="18"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="18">
+      <c r="C27" s="16">
         <v>8</v>
       </c>
-      <c r="G27" s="18"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="G29" s="18">
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
+      <c r="G29" s="16">
         <v>14</v>
       </c>
-      <c r="H29" s="20"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" s="18"/>
+        <v>28</v>
+      </c>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="18">
+      <c r="B31" s="16">
         <v>4</v>
       </c>
-      <c r="G31" s="18"/>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" spans="2:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="18"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="25"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="23"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16"/>
     </row>
     <row r="34" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="25"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="23"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="24" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="22" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="D36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
     </row>
     <row r="37" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="18"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="18"/>
+      <c r="D37" s="16"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="16"/>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="29" t="s">
+      <c r="A38" s="22"/>
+      <c r="B38" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="18"/>
+      <c r="D38" s="16"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="17"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="18"/>
-      <c r="D40" s="18">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16">
         <v>9</v>
       </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18">
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16">
         <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
+      <c r="A42" s="22"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
     </row>
     <row r="43" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="18">
+      <c r="C43" s="16">
         <v>5</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
+      <c r="C44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
     </row>
     <row r="45" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="18"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
     </row>
     <row r="46" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
-      <c r="B46" s="29" t="s">
+      <c r="A46" s="22"/>
+      <c r="B46" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
     </row>
     <row r="47" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E47" s="18"/>
+      <c r="E47" s="16"/>
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E48" s="4">
         <v>12</v>
       </c>
-      <c r="F48" s="30"/>
+      <c r="F48" s="26"/>
     </row>
     <row r="49" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F49" s="30"/>
+      <c r="F49" s="26"/>
     </row>
     <row r="50" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="24"/>
-      <c r="B50" s="25" t="s">
+      <c r="A50" s="22"/>
+      <c r="B50" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E50" s="18"/>
+      <c r="E50" s="16"/>
     </row>
     <row r="51" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="22" t="s">
         <v>5</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="E51" s="16"/>
     </row>
     <row r="52" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="17"/>
-      <c r="E52" s="31"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="18"/>
-      <c r="E53" s="31"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="27"/>
     </row>
     <row r="54" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="24"/>
-      <c r="B54" s="29" t="s">
+      <c r="A54" s="22"/>
+      <c r="B54" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C54" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="16"/>
+      <c r="E54" s="27"/>
+    </row>
+    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="15"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="16"/>
+      <c r="D56" s="16">
+        <v>10</v>
+      </c>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+    </row>
+    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+    </row>
+    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="22"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="16"/>
+    </row>
+    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="16"/>
+    </row>
+    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="22"/>
+      <c r="B62" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D54" s="18"/>
-      <c r="E54" s="31"/>
-    </row>
-    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="17"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="18"/>
-      <c r="D56" s="18">
-        <v>10</v>
-      </c>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-    </row>
-    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-    </row>
-    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="24"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="18"/>
-    </row>
-    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C61" s="18"/>
-    </row>
-    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="24"/>
-      <c r="B62" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="63" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
     </row>
     <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-    </row>
-    <row r="65" spans="1:8" s="14" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+    </row>
+    <row r="65" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="30"/>
     </row>
     <row r="66" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="33"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
+      <c r="A66" s="29"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="30"/>
     </row>
     <row r="67" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Fixed date formats and updated charts
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC09F34-B625-411B-A5B1-CF6F238ED331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB3A4D4-798E-4D20-B5DA-DA14526ACFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -386,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -442,6 +443,12 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="A13" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="I37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -810,25 +817,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -1059,17 +1066,17 @@
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="38"/>
-      <c r="B35" s="38"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="22"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="36"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="21" t="s">
         <v>6</v>
       </c>
@@ -1265,45 +1272,45 @@
       </c>
     </row>
     <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="35"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
     </row>
     <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="35"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
     </row>
     <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="35"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="35"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
     </row>
     <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="28"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="35"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1317,4 +1324,533 @@
   <pageMargins left="0.25" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2329AE-8E4E-42E7-B08B-4E199AF74E76}">
+  <dimension ref="A1:I68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.75" style="11" customWidth="1"/>
+    <col min="2" max="7" width="12.25" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="17.375" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="36"/>
+      <c r="B3" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="15"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="16"/>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="16">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="16"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="16"/>
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="17">
+        <v>7</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="16"/>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="16"/>
+      <c r="F18" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="16">
+        <v>11</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="16"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="16"/>
+      <c r="C23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="16">
+        <v>3</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="E24" s="16"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="16"/>
+      <c r="D27" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="16">
+        <v>8</v>
+      </c>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="G30" s="16">
+        <v>14</v>
+      </c>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="16"/>
+      <c r="C31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="16">
+        <v>4</v>
+      </c>
+      <c r="G32" s="16"/>
+    </row>
+    <row r="33" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="22"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="16"/>
+    </row>
+    <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="22"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="38"/>
+      <c r="C36" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+    </row>
+    <row r="37" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="16"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="16"/>
+    </row>
+    <row r="39" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="16"/>
+    </row>
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="15"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+    </row>
+    <row r="41" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="16"/>
+      <c r="D41" s="16">
+        <v>9</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="21"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+    </row>
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="16">
+        <v>5</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+    </row>
+    <row r="45" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+    </row>
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="16"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+    </row>
+    <row r="47" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="21"/>
+      <c r="B47" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+    </row>
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="16"/>
+      <c r="F48" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E49" s="4">
+        <v>12</v>
+      </c>
+      <c r="F49" s="25"/>
+    </row>
+    <row r="50" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="25"/>
+    </row>
+    <row r="51" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="16"/>
+    </row>
+    <row r="52" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="16"/>
+    </row>
+    <row r="53" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="15"/>
+      <c r="E53" s="26"/>
+    </row>
+    <row r="54" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="16"/>
+      <c r="E54" s="26"/>
+    </row>
+    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21"/>
+      <c r="B55" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="16"/>
+      <c r="E55" s="26"/>
+    </row>
+    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="15"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="16"/>
+      <c r="D57" s="16">
+        <v>10</v>
+      </c>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+    </row>
+    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+    </row>
+    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="21"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="16"/>
+    </row>
+    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="16"/>
+    </row>
+    <row r="63" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="21"/>
+      <c r="B63" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+    </row>
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+    </row>
+    <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+    </row>
+    <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="28"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+    </row>
+    <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C64:H68"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update codes and tournament table
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB3A4D4-798E-4D20-B5DA-DA14526ACFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F6B60D-8C36-4098-87E5-303373F4748D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -174,6 +175,38 @@
   </si>
   <si>
     <t>总冠军！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金贝贝(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌咪(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莎拉公主(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">沙隆巴斯(4)  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小丹尼(5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孙小美(6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忍太郎(7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钱夫人(8)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -452,6 +485,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,6 +500,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -817,25 +858,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -1066,17 +1107,17 @@
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40"/>
+      <c r="A35" s="42"/>
+      <c r="B35" s="42"/>
       <c r="C35" s="22"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="21" t="s">
         <v>6</v>
       </c>
@@ -1272,45 +1313,45 @@
       </c>
     </row>
     <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="37"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
     </row>
     <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="39"/>
     </row>
     <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="37"/>
-      <c r="H66" s="37"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="39"/>
     </row>
     <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="28"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="39"/>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="37"/>
-      <c r="H68" s="37"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1330,11 +1371,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2329AE-8E4E-42E7-B08B-4E199AF74E76}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.75" style="11" customWidth="1"/>
     <col min="2" max="7" width="12.25" style="11" customWidth="1"/>
@@ -1346,25 +1387,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -1386,7 +1427,7 @@
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -1397,9 +1438,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="16"/>
-      <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="C7" s="6"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -1410,8 +1449,8 @@
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>11</v>
+      <c r="B9" s="43" t="s">
+        <v>46</v>
       </c>
       <c r="C9" s="16"/>
       <c r="F9" s="14"/>
@@ -1422,9 +1461,6 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="16"/>
-      <c r="D11" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -1437,7 +1473,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C13" s="16"/>
       <c r="E13" s="16"/>
@@ -1450,9 +1486,7 @@
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16"/>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="E15" s="16"/>
       <c r="F15" s="19"/>
     </row>
@@ -1464,17 +1498,15 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>13</v>
+      <c r="B17" s="43" t="s">
+        <v>47</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="16"/>
-      <c r="F18" s="32" t="s">
-        <v>38</v>
-      </c>
+      <c r="F18" s="32"/>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -1489,8 +1521,8 @@
       <c r="G20" s="16"/>
     </row>
     <row r="21" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
-        <v>14</v>
+      <c r="B21" s="44" t="s">
+        <v>42</v>
       </c>
       <c r="E21" s="16"/>
       <c r="G21" s="16"/>
@@ -1502,9 +1534,7 @@
     </row>
     <row r="23" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="16"/>
-      <c r="C23" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="C23" s="6"/>
       <c r="E23" s="16"/>
       <c r="G23" s="16"/>
     </row>
@@ -1518,7 +1548,7 @@
     </row>
     <row r="25" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C25" s="16"/>
       <c r="E25" s="16"/>
@@ -1531,9 +1561,7 @@
     </row>
     <row r="27" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="16"/>
-      <c r="D27" s="33" t="s">
-        <v>32</v>
-      </c>
+      <c r="D27" s="33"/>
       <c r="E27" s="5"/>
       <c r="G27" s="16"/>
     </row>
@@ -1544,14 +1572,11 @@
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="6" t="s">
-        <v>16</v>
+      <c r="B29" s="44" t="s">
+        <v>41</v>
       </c>
       <c r="C29" s="16"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="I29" s="8" t="s">
         <v>40</v>
       </c>
@@ -1566,9 +1591,7 @@
     </row>
     <row r="31" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="16"/>
-      <c r="C31" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="C31" s="3"/>
       <c r="G31" s="16"/>
     </row>
     <row r="32" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -1579,14 +1602,12 @@
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="E33" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="F33" s="6"/>
       <c r="G33" s="16"/>
     </row>
     <row r="34" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -1595,23 +1616,21 @@
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40"/>
+      <c r="A35" s="42"/>
+      <c r="B35" s="42"/>
       <c r="C35" s="22"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="D36" s="8"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
     </row>
@@ -1630,9 +1649,6 @@
       <c r="B39" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="D39" s="16"/>
       <c r="F39" s="23"/>
       <c r="G39" s="16"/>
@@ -1640,9 +1656,7 @@
     <row r="40" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
-      <c r="E40" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="E40" s="7"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
     </row>
@@ -1653,9 +1667,7 @@
       </c>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="34" t="s">
-        <v>37</v>
-      </c>
+      <c r="G41" s="34"/>
     </row>
     <row r="42" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="16"/>
@@ -1668,9 +1680,7 @@
     <row r="43" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21"/>
       <c r="C43" s="16"/>
-      <c r="D43" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
     </row>
@@ -1698,17 +1708,13 @@
       <c r="B47" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C47" s="2"/>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
     </row>
     <row r="48" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E48" s="16"/>
-      <c r="F48" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E49" s="4">
@@ -1730,9 +1736,7 @@
       <c r="C52" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="D52" s="6"/>
       <c r="E52" s="16"/>
     </row>
     <row r="53" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -1748,18 +1752,13 @@
       <c r="B55" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="D55" s="16"/>
       <c r="E55" s="26"/>
     </row>
     <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="15"/>
       <c r="D56" s="16"/>
-      <c r="E56" s="34" t="s">
-        <v>34</v>
-      </c>
+      <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="16"/>
@@ -1776,9 +1775,7 @@
     <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="21"/>
       <c r="C59" s="16"/>
-      <c r="D59" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="16">
@@ -1796,50 +1793,514 @@
       <c r="B63" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="37"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
     </row>
     <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="39"/>
     </row>
     <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="37"/>
-      <c r="H66" s="37"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="39"/>
     </row>
     <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="28"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="39"/>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="37"/>
-      <c r="H68" s="37"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C64:H68"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC41AD02-D213-4B8C-8C48-D69FD6AD7D98}">
+  <dimension ref="A1:I68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.75" style="11" customWidth="1"/>
+    <col min="2" max="7" width="12.25" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="17.375" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="38"/>
+      <c r="B3" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="15"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="16"/>
+      <c r="C7" s="6"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="16">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="43"/>
+      <c r="C9" s="16"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="16"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="16"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="17">
+        <v>7</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="C13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="16"/>
+      <c r="C15" s="3"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="43"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="16"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="16">
+        <v>11</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="16"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="6"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="16"/>
+      <c r="C23" s="6"/>
+      <c r="E23" s="16"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="16">
+        <v>3</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="E24" s="16"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="5"/>
+      <c r="C25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="16"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="5"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="16">
+        <v>8</v>
+      </c>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6"/>
+      <c r="C29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="I29" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="G30" s="16">
+        <v>14</v>
+      </c>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="16"/>
+      <c r="C31" s="3"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="16">
+        <v>4</v>
+      </c>
+      <c r="G32" s="16"/>
+    </row>
+    <row r="33" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="5"/>
+      <c r="E33" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="22"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="16"/>
+    </row>
+    <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="42"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="22"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="40"/>
+      <c r="C36" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+    </row>
+    <row r="37" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="16"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="16"/>
+    </row>
+    <row r="39" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="16"/>
+    </row>
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="15"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+    </row>
+    <row r="41" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="16"/>
+      <c r="D41" s="16">
+        <v>9</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="21"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+    </row>
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="16">
+        <v>5</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+    </row>
+    <row r="45" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+    </row>
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="16"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+    </row>
+    <row r="47" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="21"/>
+      <c r="B47" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+    </row>
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="16"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E49" s="4">
+        <v>12</v>
+      </c>
+      <c r="F49" s="25"/>
+    </row>
+    <row r="50" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="25"/>
+    </row>
+    <row r="51" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="16"/>
+    </row>
+    <row r="52" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="16"/>
+    </row>
+    <row r="53" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="15"/>
+      <c r="E53" s="26"/>
+    </row>
+    <row r="54" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="16"/>
+      <c r="E54" s="26"/>
+    </row>
+    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21"/>
+      <c r="B55" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="16"/>
+      <c r="E55" s="26"/>
+    </row>
+    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="15"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="34"/>
+    </row>
+    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="16"/>
+      <c r="D57" s="16">
+        <v>10</v>
+      </c>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+    </row>
+    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+    </row>
+    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="21"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="16"/>
+    </row>
+    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="16"/>
+    </row>
+    <row r="63" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="21"/>
+      <c r="B63" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
+    </row>
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="39"/>
+    </row>
+    <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="39"/>
+    </row>
+    <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="28"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="39"/>
+    </row>
+    <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Updates on knockout ranking
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DFA380-692B-4AA9-9042-769DA98FD9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5D8FB6-4078-4F87-9FF6-317D19867550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -182,10 +182,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>小丹尼(5)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>孙小美(6)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -246,10 +242,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>忍太郎(7)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>第七名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -283,6 +275,30 @@
   </si>
   <si>
     <t>L10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌咪(2)   2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">乌咪(2)  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙隆巴斯(4)   3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莎拉公主(3)   0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钱夫人(8)   2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">小丹尼(5) </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -620,6 +636,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,15 +668,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1009,25 +1025,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -1258,17 +1274,17 @@
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="71"/>
-      <c r="B35" s="71"/>
+      <c r="A35" s="74"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="22"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="69" t="s">
+      <c r="A36" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="69"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="21" t="s">
         <v>6</v>
       </c>
@@ -1464,45 +1480,45 @@
       </c>
     </row>
     <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="68"/>
-      <c r="D64" s="68"/>
-      <c r="E64" s="68"/>
-      <c r="F64" s="68"/>
-      <c r="G64" s="68"/>
-      <c r="H64" s="68"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="71"/>
+      <c r="F64" s="71"/>
+      <c r="G64" s="71"/>
+      <c r="H64" s="71"/>
     </row>
     <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="68"/>
-      <c r="D65" s="68"/>
-      <c r="E65" s="68"/>
-      <c r="F65" s="68"/>
-      <c r="G65" s="68"/>
-      <c r="H65" s="68"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
     </row>
     <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="68"/>
-      <c r="D66" s="68"/>
-      <c r="E66" s="68"/>
-      <c r="F66" s="68"/>
-      <c r="G66" s="68"/>
-      <c r="H66" s="68"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="71"/>
+      <c r="E66" s="71"/>
+      <c r="F66" s="71"/>
+      <c r="G66" s="71"/>
+      <c r="H66" s="71"/>
     </row>
     <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="28"/>
-      <c r="C67" s="68"/>
-      <c r="D67" s="68"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="68"/>
-      <c r="H67" s="68"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="71"/>
+      <c r="E67" s="71"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="71"/>
+      <c r="H67" s="71"/>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C68" s="68"/>
-      <c r="D68" s="68"/>
-      <c r="E68" s="68"/>
-      <c r="F68" s="68"/>
-      <c r="G68" s="68"/>
-      <c r="H68" s="68"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="71"/>
+      <c r="E68" s="71"/>
+      <c r="F68" s="71"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1522,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2329AE-8E4E-42E7-B08B-4E199AF74E76}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:F89"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -1538,25 +1554,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -1586,7 +1602,7 @@
     <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36"/>
       <c r="B5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -1610,8 +1626,8 @@
     <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
       <c r="B7" s="43"/>
-      <c r="C7" s="36" t="s">
-        <v>47</v>
+      <c r="C7" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36"/>
@@ -1636,7 +1652,7 @@
     <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36"/>
       <c r="B9" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="43"/>
       <c r="D9" s="36"/>
@@ -1661,7 +1677,9 @@
       <c r="A11" s="36"/>
       <c r="B11" s="36"/>
       <c r="C11" s="43"/>
-      <c r="D11" s="36"/>
+      <c r="D11" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="E11" s="36"/>
       <c r="F11" s="14"/>
       <c r="G11" s="36"/>
@@ -1684,7 +1702,7 @@
     <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36"/>
       <c r="B13" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="36"/>
@@ -1709,7 +1727,7 @@
       <c r="A15" s="36"/>
       <c r="B15" s="43"/>
       <c r="C15" s="47" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="D15" s="36"/>
       <c r="E15" s="43"/>
@@ -1734,7 +1752,7 @@
     <row r="17" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
       <c r="B17" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -1782,7 +1800,7 @@
     <row r="21" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36"/>
       <c r="B21" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
@@ -1807,7 +1825,7 @@
       <c r="A23" s="36"/>
       <c r="B23" s="43"/>
       <c r="C23" s="36" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D23" s="36"/>
       <c r="E23" s="43"/>
@@ -1832,7 +1850,7 @@
     <row r="25" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="36"/>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="43"/>
       <c r="D25" s="36"/>
@@ -1857,7 +1875,9 @@
       <c r="A27" s="36"/>
       <c r="B27" s="36"/>
       <c r="C27" s="43"/>
-      <c r="D27" s="50"/>
+      <c r="D27" s="50" t="s">
+        <v>71</v>
+      </c>
       <c r="E27" s="35"/>
       <c r="F27" s="36"/>
       <c r="G27" s="43"/>
@@ -1880,7 +1900,7 @@
     <row r="29" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="36"/>
       <c r="B29" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="43"/>
       <c r="D29" s="36"/>
@@ -1908,8 +1928,8 @@
     <row r="31" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="36"/>
       <c r="B31" s="43"/>
-      <c r="C31" s="47" t="s">
-        <v>42</v>
+      <c r="C31" s="34" t="s">
+        <v>52</v>
       </c>
       <c r="D31" s="36"/>
       <c r="E31" s="36"/>
@@ -1934,7 +1954,7 @@
     <row r="33" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="36"/>
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="36"/>
       <c r="D33" s="36"/>
@@ -1958,8 +1978,8 @@
       <c r="I34" s="36"/>
     </row>
     <row r="35" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="72"/>
-      <c r="B35" s="72"/>
+      <c r="A35" s="75"/>
+      <c r="B35" s="75"/>
       <c r="C35" s="36"/>
       <c r="D35" s="36"/>
       <c r="E35" s="36"/>
@@ -1971,12 +1991,14 @@
     <row r="36" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="61"/>
       <c r="B36" s="62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="48"/>
+      <c r="D36" s="48" t="s">
+        <v>43</v>
+      </c>
       <c r="E36" s="36"/>
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
@@ -2011,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" s="43"/>
       <c r="E39" s="36"/>
@@ -2062,7 +2084,7 @@
       <c r="B43" s="36"/>
       <c r="C43" s="43"/>
       <c r="D43" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
@@ -2111,7 +2133,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" s="36"/>
       <c r="E47" s="43"/>
@@ -2172,7 +2194,9 @@
       <c r="C52" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="36"/>
+      <c r="D52" s="36" t="s">
+        <v>41</v>
+      </c>
       <c r="E52" s="43"/>
       <c r="F52" s="36"/>
       <c r="G52" s="36"/>
@@ -2207,7 +2231,7 @@
         <v>3</v>
       </c>
       <c r="C55" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D55" s="43"/>
       <c r="E55" s="55"/>
@@ -2256,7 +2280,7 @@
       <c r="B59" s="36"/>
       <c r="C59" s="43"/>
       <c r="D59" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E59" s="36"/>
       <c r="F59" s="36"/>
@@ -2305,7 +2329,7 @@
         <v>4</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D63" s="36"/>
       <c r="E63" s="36"/>
@@ -2339,10 +2363,10 @@
     <row r="66" spans="1:9" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="41"/>
       <c r="B66" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="C66" s="78" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="C66" s="70" t="s">
+        <v>64</v>
       </c>
       <c r="D66" s="48"/>
       <c r="E66" s="64"/>
@@ -2353,7 +2377,7 @@
     </row>
     <row r="67" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="57"/>
-      <c r="C67" s="77"/>
+      <c r="C67" s="69"/>
       <c r="D67" s="42"/>
       <c r="E67" s="64"/>
       <c r="F67" s="64"/>
@@ -2384,7 +2408,7 @@
       <c r="D70" s="16"/>
       <c r="E70" s="7"/>
       <c r="F70" s="65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G70" s="64"/>
       <c r="H70" s="58"/>
@@ -2412,8 +2436,8 @@
       <c r="G73" s="65"/>
     </row>
     <row r="74" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C74" s="77" t="s">
-        <v>67</v>
+      <c r="C74" s="69" t="s">
+        <v>65</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="65"/>
@@ -2438,7 +2462,7 @@
     </row>
     <row r="79" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="66" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C79" s="58"/>
       <c r="D79" s="58"/>
@@ -2446,11 +2470,11 @@
       <c r="G79" s="65"/>
     </row>
     <row r="80" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="76" t="s">
-        <v>64</v>
+      <c r="B80" s="68" t="s">
+        <v>62</v>
       </c>
       <c r="C80" s="48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D80" s="64"/>
       <c r="E80" s="64"/>
@@ -2473,9 +2497,11 @@
     </row>
     <row r="84" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C84" s="16"/>
-      <c r="D84" s="7"/>
+      <c r="D84" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="E84" s="65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="85" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -2494,10 +2520,12 @@
       <c r="E87" s="65"/>
     </row>
     <row r="88" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="C88" s="5"/>
+      <c r="B88" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="D88" s="65"/>
       <c r="E88" s="65"/>
     </row>
@@ -2519,8 +2547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC41AD02-D213-4B8C-8C48-D69FD6AD7D98}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -2535,25 +2563,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="59"/>
       <c r="B1" s="40"/>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
       <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
       <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -2741,16 +2769,16 @@
       <c r="G34" s="43"/>
     </row>
     <row r="35" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="72"/>
-      <c r="B35" s="72"/>
+      <c r="A35" s="75"/>
+      <c r="B35" s="75"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
     </row>
     <row r="36" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="75" t="s">
+      <c r="A36" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="75"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="51" t="s">
         <v>6</v>
       </c>
@@ -2943,10 +2971,10 @@
     <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="57"/>
       <c r="B67" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="C67" s="78" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="C67" s="70" t="s">
+        <v>64</v>
       </c>
       <c r="D67" s="48"/>
       <c r="E67" s="64"/>
@@ -2955,7 +2983,7 @@
     </row>
     <row r="68" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B68" s="11"/>
-      <c r="C68" s="77"/>
+      <c r="C68" s="69"/>
       <c r="D68" s="42"/>
       <c r="E68" s="64"/>
       <c r="F68" s="64"/>
@@ -2981,7 +3009,7 @@
       <c r="D71" s="16"/>
       <c r="E71" s="7"/>
       <c r="F71" s="65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -3007,8 +3035,8 @@
     </row>
     <row r="75" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="11"/>
-      <c r="C75" s="77" t="s">
-        <v>67</v>
+      <c r="C75" s="69" t="s">
+        <v>65</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="65"/>
@@ -3044,13 +3072,13 @@
     </row>
     <row r="80" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="66" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F80" s="11"/>
     </row>
     <row r="81" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="76" t="s">
-        <v>64</v>
+      <c r="B81" s="68" t="s">
+        <v>62</v>
       </c>
       <c r="C81" s="48"/>
       <c r="D81" s="64"/>
@@ -3082,7 +3110,7 @@
       <c r="C85" s="16"/>
       <c r="D85" s="7"/>
       <c r="E85" s="65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F85" s="11"/>
     </row>
@@ -3108,8 +3136,8 @@
       <c r="F88" s="11"/>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B89" s="77" t="s">
-        <v>65</v>
+      <c r="B89" s="69" t="s">
+        <v>63</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="65"/>

</xml_diff>

<commit_message>
Add knockout draw rules
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F1A1B4-7C7E-4D6E-B1BA-23CC8A416A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE005AB2-9D62-4C43-9BB4-1F5297FC6660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -331,6 +331,38 @@
   </si>
   <si>
     <t>沙隆巴斯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金贝贝(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿土伯(7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钱夫人(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小丹尼(5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙隆巴斯(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宫本宝藏(8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忍太郎(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莎拉公主(6)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -557,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -689,6 +721,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -713,7 +752,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1070,25 +1108,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -1319,17 +1357,17 @@
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="78"/>
-      <c r="B35" s="78"/>
+      <c r="A35" s="81"/>
+      <c r="B35" s="81"/>
       <c r="C35" s="22"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="76" t="s">
+      <c r="A36" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="76"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="21" t="s">
         <v>6</v>
       </c>
@@ -1525,45 +1563,45 @@
       </c>
     </row>
     <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="75"/>
-      <c r="H64" s="75"/>
+      <c r="C64" s="78"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="78"/>
+      <c r="F64" s="78"/>
+      <c r="G64" s="78"/>
+      <c r="H64" s="78"/>
     </row>
     <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
+      <c r="C65" s="78"/>
+      <c r="D65" s="78"/>
+      <c r="E65" s="78"/>
+      <c r="F65" s="78"/>
+      <c r="G65" s="78"/>
+      <c r="H65" s="78"/>
     </row>
     <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
+      <c r="C66" s="78"/>
+      <c r="D66" s="78"/>
+      <c r="E66" s="78"/>
+      <c r="F66" s="78"/>
+      <c r="G66" s="78"/>
+      <c r="H66" s="78"/>
     </row>
     <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="28"/>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
+      <c r="C67" s="78"/>
+      <c r="D67" s="78"/>
+      <c r="E67" s="78"/>
+      <c r="F67" s="78"/>
+      <c r="G67" s="78"/>
+      <c r="H67" s="78"/>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
+      <c r="C68" s="78"/>
+      <c r="D68" s="78"/>
+      <c r="E68" s="78"/>
+      <c r="F68" s="78"/>
+      <c r="G68" s="78"/>
+      <c r="H68" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1583,7 +1621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2329AE-8E4E-42E7-B08B-4E199AF74E76}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -1599,25 +1637,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -1816,7 +1854,7 @@
       <c r="D18" s="36"/>
       <c r="E18" s="43"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="83" t="s">
+      <c r="G18" s="77" t="s">
         <v>64</v>
       </c>
       <c r="H18" s="36"/>
@@ -2033,8 +2071,8 @@
       <c r="I34" s="36"/>
     </row>
     <row r="35" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="79"/>
-      <c r="B35" s="79"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="36"/>
       <c r="D35" s="36"/>
       <c r="E35" s="36"/>
@@ -2616,8 +2654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC41AD02-D213-4B8C-8C48-D69FD6AD7D98}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -2632,38 +2670,38 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="59"/>
       <c r="B1" s="40"/>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
       <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="37"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
       <c r="I3" s="40"/>
     </row>
     <row r="4" spans="1:9" s="41" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -2671,6 +2709,9 @@
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="s">
+        <v>80</v>
+      </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
@@ -2690,7 +2731,9 @@
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35"/>
+      <c r="B9" s="35" t="s">
+        <v>81</v>
+      </c>
       <c r="C9" s="43"/>
       <c r="F9" s="14"/>
     </row>
@@ -2711,7 +2754,9 @@
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="46"/>
+      <c r="B13" s="46" t="s">
+        <v>82</v>
+      </c>
       <c r="C13" s="43"/>
       <c r="E13" s="43"/>
     </row>
@@ -2735,7 +2780,9 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="2:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="35"/>
+      <c r="B17" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="E17" s="43"/>
       <c r="F17" s="19"/>
     </row>
@@ -2756,6 +2803,9 @@
       <c r="G20" s="43"/>
     </row>
     <row r="21" spans="2:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="E21" s="43"/>
       <c r="G21" s="43"/>
     </row>
@@ -2778,7 +2828,9 @@
       <c r="G24" s="43"/>
     </row>
     <row r="25" spans="2:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>85</v>
+      </c>
       <c r="C25" s="43"/>
       <c r="E25" s="43"/>
       <c r="G25" s="43"/>
@@ -2801,6 +2853,9 @@
       <c r="G28" s="43"/>
     </row>
     <row r="29" spans="2:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="C29" s="43"/>
       <c r="G29" s="43"/>
       <c r="I29" s="48" t="s">
@@ -2827,7 +2882,9 @@
       <c r="G32" s="43"/>
     </row>
     <row r="33" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="35"/>
+      <c r="B33" s="35" t="s">
+        <v>87</v>
+      </c>
       <c r="E33" s="51" t="s">
         <v>73</v>
       </c>
@@ -2838,16 +2895,16 @@
       <c r="G34" s="43"/>
     </row>
     <row r="35" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="79"/>
-      <c r="B35" s="79"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="82"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
     </row>
     <row r="36" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="82"/>
+      <c r="B36" s="85"/>
       <c r="C36" s="51" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
update on the 4th tournament
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639B2E06-C691-4739-8697-155760BBFEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0BAF05-9B41-46A4-BEBF-99EE178A3AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="104">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -653,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -800,6 +801,15 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,9 +832,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1171,40 +1178,40 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.36328125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="11" customWidth="1"/>
-    <col min="2" max="7" width="12.25" style="11" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="11" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="17.375" style="11"/>
+    <col min="1" max="1" width="2.7265625" style="11" customWidth="1"/>
+    <col min="2" max="7" width="12.26953125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="17.36328125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
+    <row r="2" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="30"/>
       <c r="B3" s="31" t="s">
         <v>26</v>
@@ -1217,54 +1224,54 @@
       <c r="H3" s="29"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="12" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="16"/>
       <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="16">
         <v>1</v>
       </c>
       <c r="C8" s="15"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="16"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="16"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="16"/>
       <c r="D11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="17">
         <v>7</v>
       </c>
@@ -1272,20 +1279,20 @@
       <c r="E12" s="15"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="16"/>
       <c r="C15" s="3" t="s">
         <v>23</v>
@@ -1293,51 +1300,51 @@
       <c r="E15" s="16"/>
       <c r="F15" s="19"/>
     </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="16">
         <v>2</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="19"/>
     </row>
-    <row r="17" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="19"/>
     </row>
-    <row r="18" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="16"/>
       <c r="F18" s="32" t="s">
         <v>38</v>
       </c>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E19" s="16">
         <v>11</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
       <c r="E22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="16"/>
       <c r="C23" s="6" t="s">
         <v>24</v>
@@ -1345,7 +1352,7 @@
       <c r="E23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="16">
         <v>3</v>
       </c>
@@ -1353,7 +1360,7 @@
       <c r="E24" s="16"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
@@ -1361,12 +1368,12 @@
       <c r="E25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="16"/>
       <c r="E26" s="16"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="16"/>
       <c r="D27" s="33" t="s">
         <v>32</v>
@@ -1374,13 +1381,13 @@
       <c r="E27" s="5"/>
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="16">
         <v>8</v>
       </c>
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>16</v>
       </c>
@@ -1393,7 +1400,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="15"/>
       <c r="C30" s="16"/>
       <c r="G30" s="16">
@@ -1401,20 +1408,20 @@
       </c>
       <c r="H30" s="18"/>
     </row>
-    <row r="31" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="16"/>
       <c r="C31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G31" s="16"/>
     </row>
-    <row r="32" spans="2:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="16">
         <v>4</v>
       </c>
       <c r="G32" s="16"/>
     </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
@@ -1426,23 +1433,23 @@
       </c>
       <c r="G33" s="16"/>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="22"/>
       <c r="F34" s="15"/>
       <c r="G34" s="16"/>
     </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="83"/>
-      <c r="B35" s="83"/>
+    <row r="35" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="86"/>
+      <c r="B35" s="86"/>
       <c r="C35" s="22"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
     </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="81" t="s">
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="81"/>
+      <c r="B36" s="84"/>
       <c r="C36" s="21" t="s">
         <v>6</v>
       </c>
@@ -1452,17 +1459,17 @@
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
     </row>
-    <row r="37" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="16"/>
       <c r="F38" s="23"/>
       <c r="G38" s="16"/>
     </row>
-    <row r="39" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21"/>
       <c r="B39" s="24" t="s">
         <v>1</v>
@@ -1474,7 +1481,7 @@
       <c r="F39" s="23"/>
       <c r="G39" s="16"/>
     </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
       <c r="E40" s="7" t="s">
@@ -1483,7 +1490,7 @@
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
     </row>
-    <row r="41" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="16"/>
       <c r="D41" s="16">
         <v>9</v>
@@ -1494,7 +1501,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -1502,7 +1509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21"/>
       <c r="C43" s="16"/>
       <c r="D43" s="2" t="s">
@@ -1511,7 +1518,7 @@
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="16">
         <v>5</v>
       </c>
@@ -1519,18 +1526,18 @@
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
     </row>
-    <row r="45" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="16"/>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
     </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="16"/>
       <c r="D46" s="25"/>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
     </row>
-    <row r="47" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="21"/>
       <c r="B47" s="24" t="s">
         <v>2</v>
@@ -1541,29 +1548,29 @@
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
     </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E48" s="16"/>
       <c r="F48" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E49" s="4">
         <v>12</v>
       </c>
       <c r="F49" s="25"/>
     </row>
-    <row r="50" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F50" s="25"/>
     </row>
-    <row r="51" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="21"/>
       <c r="B51" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E51" s="16"/>
     </row>
-    <row r="52" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="21" t="s">
         <v>5</v>
       </c>
@@ -1572,15 +1579,15 @@
       </c>
       <c r="E52" s="16"/>
     </row>
-    <row r="53" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D53" s="15"/>
       <c r="E53" s="26"/>
     </row>
-    <row r="54" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D54" s="16"/>
       <c r="E54" s="26"/>
     </row>
-    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="21"/>
       <c r="B55" s="24" t="s">
         <v>3</v>
@@ -1591,14 +1598,14 @@
       <c r="D55" s="16"/>
       <c r="E55" s="26"/>
     </row>
-    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="15"/>
       <c r="D56" s="16"/>
       <c r="E56" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="16"/>
       <c r="D57" s="16">
         <v>10</v>
@@ -1606,29 +1613,29 @@
       <c r="H57" s="27"/>
       <c r="I57" s="27"/>
     </row>
-    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
     </row>
-    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="21"/>
       <c r="C59" s="16"/>
       <c r="D59" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="16">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="16"/>
     </row>
-    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="16"/>
     </row>
-    <row r="63" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="21"/>
       <c r="B63" s="24" t="s">
         <v>4</v>
@@ -1637,46 +1644,46 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="80"/>
-      <c r="D64" s="80"/>
-      <c r="E64" s="80"/>
-      <c r="F64" s="80"/>
-      <c r="G64" s="80"/>
-      <c r="H64" s="80"/>
-    </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="80"/>
-      <c r="D65" s="80"/>
-      <c r="E65" s="80"/>
-      <c r="F65" s="80"/>
-      <c r="G65" s="80"/>
-      <c r="H65" s="80"/>
-    </row>
-    <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="80"/>
-      <c r="D66" s="80"/>
-      <c r="E66" s="80"/>
-      <c r="F66" s="80"/>
-      <c r="G66" s="80"/>
-      <c r="H66" s="80"/>
-    </row>
-    <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="83"/>
+      <c r="D64" s="83"/>
+      <c r="E64" s="83"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="83"/>
+      <c r="H64" s="83"/>
+    </row>
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="83"/>
+      <c r="D65" s="83"/>
+      <c r="E65" s="83"/>
+      <c r="F65" s="83"/>
+      <c r="G65" s="83"/>
+      <c r="H65" s="83"/>
+    </row>
+    <row r="66" spans="1:8" s="12" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C66" s="83"/>
+      <c r="D66" s="83"/>
+      <c r="E66" s="83"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="83"/>
+      <c r="H66" s="83"/>
+    </row>
+    <row r="67" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="28"/>
-      <c r="C67" s="80"/>
-      <c r="D67" s="80"/>
-      <c r="E67" s="80"/>
-      <c r="F67" s="80"/>
-      <c r="G67" s="80"/>
-      <c r="H67" s="80"/>
-    </row>
-    <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C68" s="80"/>
-      <c r="D68" s="80"/>
-      <c r="E68" s="80"/>
-      <c r="F68" s="80"/>
-      <c r="G68" s="80"/>
-      <c r="H68" s="80"/>
+      <c r="C67" s="83"/>
+      <c r="D67" s="83"/>
+      <c r="E67" s="83"/>
+      <c r="F67" s="83"/>
+      <c r="G67" s="83"/>
+      <c r="H67" s="83"/>
+    </row>
+    <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C68" s="83"/>
+      <c r="D68" s="83"/>
+      <c r="E68" s="83"/>
+      <c r="F68" s="83"/>
+      <c r="G68" s="83"/>
+      <c r="H68" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1700,40 +1707,40 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.36328125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="11" customWidth="1"/>
-    <col min="2" max="7" width="12.25" style="11" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="11" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="17.375" style="11"/>
+    <col min="1" max="1" width="2.7265625" style="11" customWidth="1"/>
+    <col min="2" max="7" width="12.26953125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="17.36328125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
+    <row r="2" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="37"/>
       <c r="B3" s="38" t="s">
         <v>26</v>
@@ -1746,7 +1753,7 @@
       <c r="H3" s="39"/>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:9" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="12" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
@@ -1757,7 +1764,7 @@
       <c r="H4" s="41"/>
       <c r="I4" s="41"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36"/>
       <c r="B5" s="6" t="s">
         <v>41</v>
@@ -1770,7 +1777,7 @@
       <c r="H5" s="36"/>
       <c r="I5" s="36"/>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36"/>
       <c r="B6" s="42"/>
       <c r="C6" s="36"/>
@@ -1781,7 +1788,7 @@
       <c r="H6" s="36"/>
       <c r="I6" s="36"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="36"/>
       <c r="B7" s="43"/>
       <c r="C7" s="6" t="s">
@@ -1794,7 +1801,7 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
     </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
       <c r="B8" s="43">
         <v>1</v>
@@ -1807,7 +1814,7 @@
       <c r="H8" s="36"/>
       <c r="I8" s="36"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36"/>
       <c r="B9" s="35" t="s">
         <v>42</v>
@@ -1820,7 +1827,7 @@
       <c r="H9" s="36"/>
       <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="43"/>
@@ -1831,7 +1838,7 @@
       <c r="H10" s="36"/>
       <c r="I10" s="36"/>
     </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
       <c r="B11" s="36"/>
       <c r="C11" s="43"/>
@@ -1846,7 +1853,7 @@
       <c r="H11" s="36"/>
       <c r="I11" s="36"/>
     </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="44">
@@ -1859,7 +1866,7 @@
       <c r="H12" s="36"/>
       <c r="I12" s="36"/>
     </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36"/>
       <c r="B13" s="59" t="s">
         <v>44</v>
@@ -1872,7 +1879,7 @@
       <c r="H13" s="36"/>
       <c r="I13" s="36"/>
     </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="36"/>
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
@@ -1883,7 +1890,7 @@
       <c r="H14" s="36"/>
       <c r="I14" s="36"/>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36"/>
       <c r="B15" s="43"/>
       <c r="C15" s="46" t="s">
@@ -1896,7 +1903,7 @@
       <c r="H15" s="36"/>
       <c r="I15" s="36"/>
     </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="36"/>
       <c r="B16" s="43">
         <v>2</v>
@@ -1909,7 +1916,7 @@
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="36"/>
       <c r="B17" s="35" t="s">
         <v>45</v>
@@ -1922,7 +1929,7 @@
       <c r="H17" s="36"/>
       <c r="I17" s="36"/>
     </row>
-    <row r="18" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -1935,7 +1942,7 @@
       <c r="H18" s="36"/>
       <c r="I18" s="36"/>
     </row>
-    <row r="19" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="36"/>
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
@@ -1948,7 +1955,7 @@
       <c r="H19" s="36"/>
       <c r="I19" s="36"/>
     </row>
-    <row r="20" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -1959,7 +1966,7 @@
       <c r="H20" s="36"/>
       <c r="I20" s="36"/>
     </row>
-    <row r="21" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36"/>
       <c r="B21" s="36" t="s">
         <v>46</v>
@@ -1972,7 +1979,7 @@
       <c r="H21" s="36"/>
       <c r="I21" s="36"/>
     </row>
-    <row r="22" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36"/>
       <c r="B22" s="42"/>
       <c r="C22" s="36"/>
@@ -1983,7 +1990,7 @@
       <c r="H22" s="36"/>
       <c r="I22" s="36"/>
     </row>
-    <row r="23" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36"/>
       <c r="B23" s="43"/>
       <c r="C23" s="36" t="s">
@@ -1996,7 +2003,7 @@
       <c r="H23" s="36"/>
       <c r="I23" s="36"/>
     </row>
-    <row r="24" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="36"/>
       <c r="B24" s="43">
         <v>3</v>
@@ -2009,7 +2016,7 @@
       <c r="H24" s="36"/>
       <c r="I24" s="36"/>
     </row>
-    <row r="25" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="36"/>
       <c r="B25" s="2" t="s">
         <v>47</v>
@@ -2022,7 +2029,7 @@
       <c r="H25" s="36"/>
       <c r="I25" s="36"/>
     </row>
-    <row r="26" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="43"/>
@@ -2033,7 +2040,7 @@
       <c r="H26" s="36"/>
       <c r="I26" s="36"/>
     </row>
-    <row r="27" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="36"/>
       <c r="B27" s="36"/>
       <c r="C27" s="43"/>
@@ -2048,7 +2055,7 @@
       <c r="H27" s="36"/>
       <c r="I27" s="36"/>
     </row>
-    <row r="28" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="43">
@@ -2061,7 +2068,7 @@
       <c r="H28" s="36"/>
       <c r="I28" s="36"/>
     </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="36"/>
       <c r="B29" s="36" t="s">
         <v>48</v>
@@ -2078,7 +2085,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="36"/>
       <c r="B30" s="42"/>
       <c r="C30" s="43"/>
@@ -2091,7 +2098,7 @@
       <c r="H30" s="45"/>
       <c r="I30" s="36"/>
     </row>
-    <row r="31" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="36"/>
       <c r="B31" s="43"/>
       <c r="C31" s="34" t="s">
@@ -2104,7 +2111,7 @@
       <c r="H31" s="36"/>
       <c r="I31" s="36"/>
     </row>
-    <row r="32" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="36"/>
       <c r="B32" s="43">
         <v>4</v>
@@ -2117,7 +2124,7 @@
       <c r="H32" s="36"/>
       <c r="I32" s="36"/>
     </row>
-    <row r="33" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="36"/>
       <c r="B33" s="2" t="s">
         <v>49</v>
@@ -2134,7 +2141,7 @@
       <c r="H33" s="36"/>
       <c r="I33" s="36"/>
     </row>
-    <row r="34" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="36"/>
       <c r="B34" s="36"/>
       <c r="C34" s="36"/>
@@ -2145,9 +2152,9 @@
       <c r="H34" s="36"/>
       <c r="I34" s="36"/>
     </row>
-    <row r="35" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="84"/>
-      <c r="B35" s="84"/>
+    <row r="35" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="87"/>
+      <c r="B35" s="87"/>
       <c r="C35" s="36"/>
       <c r="D35" s="36"/>
       <c r="E35" s="36"/>
@@ -2156,7 +2163,7 @@
       <c r="H35" s="36"/>
       <c r="I35" s="36"/>
     </row>
-    <row r="36" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="60"/>
       <c r="B36" s="61" t="s">
         <v>50</v>
@@ -2173,7 +2180,7 @@
       <c r="H36" s="36"/>
       <c r="I36" s="36"/>
     </row>
-    <row r="37" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="36"/>
       <c r="B37" s="36"/>
       <c r="C37" s="36"/>
@@ -2184,7 +2191,7 @@
       <c r="H37" s="36"/>
       <c r="I37" s="36"/>
     </row>
-    <row r="38" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="36"/>
       <c r="B38" s="36"/>
       <c r="C38" s="36"/>
@@ -2195,7 +2202,7 @@
       <c r="H38" s="36"/>
       <c r="I38" s="36"/>
     </row>
-    <row r="39" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="50"/>
       <c r="B39" s="52" t="s">
         <v>1</v>
@@ -2210,7 +2217,7 @@
       <c r="H39" s="36"/>
       <c r="I39" s="36"/>
     </row>
-    <row r="40" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="36"/>
       <c r="B40" s="36"/>
       <c r="C40" s="42"/>
@@ -2223,7 +2230,7 @@
       <c r="H40" s="36"/>
       <c r="I40" s="36"/>
     </row>
-    <row r="41" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="36"/>
       <c r="B41" s="36"/>
       <c r="C41" s="43"/>
@@ -2238,7 +2245,7 @@
       <c r="H41" s="36"/>
       <c r="I41" s="36"/>
     </row>
-    <row r="42" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="36"/>
       <c r="B42" s="36"/>
       <c r="C42" s="43"/>
@@ -2251,7 +2258,7 @@
       <c r="H42" s="36"/>
       <c r="I42" s="36"/>
     </row>
-    <row r="43" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50"/>
       <c r="B43" s="36"/>
       <c r="C43" s="43"/>
@@ -2264,7 +2271,7 @@
       <c r="H43" s="36"/>
       <c r="I43" s="36"/>
     </row>
-    <row r="44" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="36"/>
       <c r="B44" s="36"/>
       <c r="C44" s="43">
@@ -2277,7 +2284,7 @@
       <c r="H44" s="36"/>
       <c r="I44" s="36"/>
     </row>
-    <row r="45" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="36"/>
       <c r="B45" s="36"/>
       <c r="C45" s="43"/>
@@ -2288,7 +2295,7 @@
       <c r="H45" s="36"/>
       <c r="I45" s="36"/>
     </row>
-    <row r="46" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="36"/>
       <c r="B46" s="36"/>
       <c r="C46" s="43"/>
@@ -2299,7 +2306,7 @@
       <c r="H46" s="36"/>
       <c r="I46" s="36"/>
     </row>
-    <row r="47" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50"/>
       <c r="B47" s="52" t="s">
         <v>2</v>
@@ -2314,7 +2321,7 @@
       <c r="H47" s="36"/>
       <c r="I47" s="36"/>
     </row>
-    <row r="48" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="36"/>
       <c r="B48" s="36"/>
       <c r="C48" s="36"/>
@@ -2327,7 +2334,7 @@
       <c r="H48" s="36"/>
       <c r="I48" s="36"/>
     </row>
-    <row r="49" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="36"/>
       <c r="B49" s="36"/>
       <c r="C49" s="36"/>
@@ -2340,7 +2347,7 @@
       <c r="H49" s="36"/>
       <c r="I49" s="36"/>
     </row>
-    <row r="50" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="36"/>
       <c r="B50" s="36"/>
       <c r="C50" s="36"/>
@@ -2351,7 +2358,7 @@
       <c r="H50" s="36"/>
       <c r="I50" s="36"/>
     </row>
-    <row r="51" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50"/>
       <c r="B51" s="36"/>
       <c r="C51" s="36"/>
@@ -2362,7 +2369,7 @@
       <c r="H51" s="36"/>
       <c r="I51" s="36"/>
     </row>
-    <row r="52" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="36"/>
       <c r="B52" s="36"/>
       <c r="C52" s="50" t="s">
@@ -2377,7 +2384,7 @@
       <c r="H52" s="36"/>
       <c r="I52" s="36"/>
     </row>
-    <row r="53" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="36"/>
       <c r="B53" s="36"/>
       <c r="C53" s="36"/>
@@ -2388,7 +2395,7 @@
       <c r="H53" s="36"/>
       <c r="I53" s="36"/>
     </row>
-    <row r="54" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="36"/>
       <c r="B54" s="36"/>
       <c r="C54" s="36"/>
@@ -2399,7 +2406,7 @@
       <c r="H54" s="36"/>
       <c r="I54" s="36"/>
     </row>
-    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="50"/>
       <c r="B55" s="52" t="s">
         <v>3</v>
@@ -2414,7 +2421,7 @@
       <c r="H55" s="36"/>
       <c r="I55" s="36"/>
     </row>
-    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="36"/>
       <c r="B56" s="36"/>
       <c r="C56" s="42"/>
@@ -2427,7 +2434,7 @@
       <c r="H56" s="36"/>
       <c r="I56" s="36"/>
     </row>
-    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="36"/>
       <c r="B57" s="36"/>
       <c r="C57" s="43"/>
@@ -2440,7 +2447,7 @@
       <c r="H57" s="55"/>
       <c r="I57" s="55"/>
     </row>
-    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="36"/>
       <c r="B58" s="36"/>
       <c r="C58" s="43"/>
@@ -2451,7 +2458,7 @@
       <c r="H58" s="36"/>
       <c r="I58" s="36"/>
     </row>
-    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="50"/>
       <c r="B59" s="36"/>
       <c r="C59" s="43"/>
@@ -2464,7 +2471,7 @@
       <c r="H59" s="36"/>
       <c r="I59" s="36"/>
     </row>
-    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="36"/>
       <c r="B60" s="36"/>
       <c r="C60" s="43">
@@ -2477,7 +2484,7 @@
       <c r="H60" s="36"/>
       <c r="I60" s="36"/>
     </row>
-    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="36"/>
       <c r="B61" s="36"/>
       <c r="C61" s="43"/>
@@ -2488,7 +2495,7 @@
       <c r="H61" s="36"/>
       <c r="I61" s="36"/>
     </row>
-    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="36"/>
       <c r="B62" s="36"/>
       <c r="C62" s="43"/>
@@ -2499,7 +2506,7 @@
       <c r="H62" s="36"/>
       <c r="I62" s="36"/>
     </row>
-    <row r="63" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="50"/>
       <c r="B63" s="52" t="s">
         <v>4</v>
@@ -2514,7 +2521,7 @@
       <c r="H63" s="36"/>
       <c r="I63" s="36"/>
     </row>
-    <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="36"/>
       <c r="B64" s="36"/>
       <c r="C64" s="40"/>
@@ -2525,7 +2532,7 @@
       <c r="H64" s="40"/>
       <c r="I64" s="36"/>
     </row>
-    <row r="65" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:9" s="4" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="36"/>
       <c r="B65" s="36"/>
       <c r="C65" s="40"/>
@@ -2536,7 +2543,7 @@
       <c r="H65" s="40"/>
       <c r="I65" s="36"/>
     </row>
-    <row r="66" spans="1:9" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:9" s="12" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="41"/>
       <c r="B66" s="66" t="s">
         <v>54</v>
@@ -2553,7 +2560,7 @@
       <c r="H66" s="40"/>
       <c r="I66" s="41"/>
     </row>
-    <row r="67" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="56"/>
       <c r="C67" s="68"/>
       <c r="D67" s="42"/>
@@ -2563,7 +2570,7 @@
       <c r="H67" s="40"/>
       <c r="I67" s="57"/>
     </row>
-    <row r="68" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="57"/>
       <c r="D68" s="16"/>
       <c r="E68" s="64"/>
@@ -2572,7 +2579,7 @@
       <c r="H68" s="40"/>
       <c r="I68" s="57"/>
     </row>
-    <row r="69" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="57"/>
       <c r="D69" s="16"/>
       <c r="E69" s="64"/>
@@ -2581,7 +2588,7 @@
       <c r="H69" s="57"/>
       <c r="I69" s="57"/>
     </row>
-    <row r="70" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="57"/>
       <c r="D70" s="16"/>
       <c r="E70" s="7" t="s">
@@ -2594,7 +2601,7 @@
       <c r="H70" s="57"/>
       <c r="I70" s="57"/>
     </row>
-    <row r="71" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="57"/>
       <c r="D71" s="62"/>
       <c r="E71" s="64"/>
@@ -2603,19 +2610,19 @@
       <c r="H71" s="57"/>
       <c r="I71" s="57"/>
     </row>
-    <row r="72" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D72" s="16"/>
       <c r="E72" s="64"/>
       <c r="F72" s="64"/>
       <c r="G72" s="64"/>
     </row>
-    <row r="73" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D73" s="16"/>
       <c r="E73" s="64"/>
       <c r="F73" s="64"/>
       <c r="G73" s="64"/>
     </row>
-    <row r="74" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C74" s="68" t="s">
         <v>61</v>
       </c>
@@ -2626,23 +2633,23 @@
       <c r="F74" s="64"/>
       <c r="G74" s="64"/>
     </row>
-    <row r="75" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C75" s="64"/>
       <c r="D75" s="64"/>
       <c r="E75" s="64"/>
       <c r="F75" s="64"/>
       <c r="G75" s="64"/>
     </row>
-    <row r="76" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G76" s="64"/>
     </row>
-    <row r="77" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G77" s="64"/>
     </row>
-    <row r="78" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G78" s="64"/>
     </row>
-    <row r="79" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="65" t="s">
         <v>55</v>
       </c>
@@ -2651,7 +2658,7 @@
       <c r="E79" s="57"/>
       <c r="G79" s="64"/>
     </row>
-    <row r="80" spans="1:9" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="67" t="s">
         <v>58</v>
       </c>
@@ -2661,23 +2668,23 @@
       <c r="D80" s="63"/>
       <c r="E80" s="63"/>
     </row>
-    <row r="81" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B81" s="57"/>
       <c r="C81" s="42"/>
       <c r="D81" s="63"/>
       <c r="E81" s="63"/>
     </row>
-    <row r="82" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C82" s="16"/>
       <c r="D82" s="64"/>
       <c r="E82" s="64"/>
     </row>
-    <row r="83" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C83" s="16"/>
       <c r="D83" s="64"/>
       <c r="E83" s="64"/>
     </row>
-    <row r="84" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C84" s="16"/>
       <c r="D84" s="7" t="s">
         <v>63</v>
@@ -2686,22 +2693,22 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C85" s="62"/>
       <c r="D85" s="64"/>
       <c r="E85" s="64"/>
     </row>
-    <row r="86" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C86" s="16"/>
       <c r="D86" s="64"/>
       <c r="E86" s="64"/>
     </row>
-    <row r="87" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C87" s="16"/>
       <c r="D87" s="64"/>
       <c r="E87" s="64"/>
     </row>
-    <row r="88" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="68" t="s">
         <v>59</v>
       </c>
@@ -2711,8 +2718,8 @@
       <c r="D88" s="64"/>
       <c r="E88" s="64"/>
     </row>
-    <row r="89" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="2:5" ht="11.9" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:H2"/>
@@ -2729,44 +2736,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC41AD02-D213-4B8C-8C48-D69FD6AD7D98}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K91" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.36328125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="57" customWidth="1"/>
-    <col min="2" max="7" width="12.25" style="57" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="57" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="57" customWidth="1"/>
-    <col min="10" max="16384" width="17.375" style="57"/>
+    <col min="1" max="1" width="2.7265625" style="57" customWidth="1"/>
+    <col min="2" max="7" width="12.26953125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="57" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" style="57" customWidth="1"/>
+    <col min="10" max="16384" width="17.36328125" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="58"/>
       <c r="B1" s="40"/>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
       <c r="I1" s="40"/>
     </row>
-    <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
+    <row r="2" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
       <c r="I2" s="40"/>
     </row>
-    <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="75"/>
       <c r="B3" s="38" t="s">
         <v>26</v>
@@ -2779,47 +2786,47 @@
       <c r="H3" s="74"/>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:9" s="41" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="41" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">
         <v>83</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="42"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="43"/>
       <c r="C7" s="36" t="s">
         <v>93</v>
       </c>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="43">
         <v>1</v>
       </c>
       <c r="C8" s="42"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C9" s="43"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="43"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="43"/>
       <c r="D11" s="36" t="s">
         <v>80</v>
@@ -2829,7 +2836,7 @@
       </c>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="44">
         <v>7</v>
       </c>
@@ -2837,20 +2844,20 @@
       <c r="E12" s="42"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="59" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="43"/>
       <c r="E13" s="43"/>
     </row>
-    <row r="14" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
       <c r="E14" s="43"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="43"/>
       <c r="C15" s="34" t="s">
         <v>85</v>
@@ -2858,51 +2865,51 @@
       <c r="E15" s="43"/>
       <c r="F15" s="19"/>
     </row>
-    <row r="16" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="43">
         <v>2</v>
       </c>
       <c r="E16" s="43"/>
       <c r="F16" s="19"/>
     </row>
-    <row r="17" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
         <v>86</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="19"/>
     </row>
-    <row r="18" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="43"/>
       <c r="F18" s="32"/>
       <c r="G18" s="76" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E19" s="43">
         <v>12</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="42"/>
     </row>
-    <row r="20" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E20" s="43"/>
       <c r="G20" s="43"/>
     </row>
-    <row r="21" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>81</v>
       </c>
       <c r="E21" s="43"/>
       <c r="G21" s="43"/>
     </row>
-    <row r="22" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="42"/>
       <c r="E22" s="43"/>
       <c r="G22" s="43"/>
     </row>
-    <row r="23" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="43"/>
       <c r="C23" s="6" t="s">
         <v>81</v>
@@ -2910,7 +2917,7 @@
       <c r="E23" s="43"/>
       <c r="G23" s="43"/>
     </row>
-    <row r="24" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="43">
         <v>3</v>
       </c>
@@ -2919,7 +2926,7 @@
       <c r="G24" s="43"/>
       <c r="I24" s="47"/>
     </row>
-    <row r="25" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="35" t="s">
         <v>82</v>
       </c>
@@ -2928,13 +2935,13 @@
       <c r="G25" s="43"/>
       <c r="I25" s="43"/>
     </row>
-    <row r="26" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="43"/>
       <c r="E26" s="43"/>
       <c r="G26" s="43"/>
       <c r="I26" s="43"/>
     </row>
-    <row r="27" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="43"/>
       <c r="D27" s="33" t="s">
         <v>95</v>
@@ -2946,21 +2953,21 @@
       <c r="I27" s="43">
         <v>15</v>
       </c>
-      <c r="J27" s="88" t="s">
+      <c r="J27" s="82" t="s">
         <v>103</v>
       </c>
       <c r="K27" s="36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="43">
         <v>8</v>
       </c>
       <c r="G28" s="43"/>
       <c r="I28" s="43"/>
     </row>
-    <row r="29" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>87</v>
       </c>
@@ -2968,7 +2975,7 @@
       <c r="G29" s="43"/>
       <c r="I29" s="35"/>
     </row>
-    <row r="30" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="42"/>
       <c r="C30" s="43"/>
       <c r="G30" s="43">
@@ -2976,20 +2983,20 @@
       </c>
       <c r="H30" s="45"/>
     </row>
-    <row r="31" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="43"/>
       <c r="C31" s="46" t="s">
         <v>94</v>
       </c>
       <c r="G31" s="43"/>
     </row>
-    <row r="32" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="43">
         <v>4</v>
       </c>
       <c r="G32" s="43"/>
     </row>
-    <row r="33" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="35" t="s">
         <v>88</v>
       </c>
@@ -3001,21 +3008,21 @@
       </c>
       <c r="G33" s="43"/>
     </row>
-    <row r="34" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F34" s="42"/>
       <c r="G34" s="43"/>
     </row>
-    <row r="35" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="84"/>
-      <c r="B35" s="84"/>
+    <row r="35" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="87"/>
+      <c r="B35" s="87"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
     </row>
-    <row r="36" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="87" t="s">
+    <row r="36" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="87"/>
+      <c r="B36" s="90"/>
       <c r="C36" s="50" t="s">
         <v>6</v>
       </c>
@@ -3025,17 +3032,17 @@
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
     </row>
-    <row r="37" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="43"/>
       <c r="F37" s="43"/>
       <c r="G37" s="43"/>
     </row>
-    <row r="38" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="43"/>
       <c r="F38" s="51"/>
       <c r="G38" s="43"/>
     </row>
-    <row r="39" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="50"/>
       <c r="B39" s="52" t="s">
         <v>1</v>
@@ -3047,7 +3054,7 @@
       <c r="F39" s="51"/>
       <c r="G39" s="43"/>
     </row>
-    <row r="40" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="42"/>
       <c r="D40" s="43"/>
       <c r="E40" s="33" t="s">
@@ -3056,7 +3063,7 @@
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
     </row>
-    <row r="41" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="43"/>
       <c r="D41" s="43">
         <v>9</v>
@@ -3067,7 +3074,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
       <c r="E42" s="43"/>
@@ -3075,7 +3082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50"/>
       <c r="C43" s="43"/>
       <c r="D43" s="2" t="s">
@@ -3084,7 +3091,7 @@
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
     </row>
-    <row r="44" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="43">
         <v>5</v>
       </c>
@@ -3092,18 +3099,18 @@
       <c r="E44" s="43"/>
       <c r="F44" s="43"/>
     </row>
-    <row r="45" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="43"/>
       <c r="E45" s="43"/>
       <c r="F45" s="43"/>
     </row>
-    <row r="46" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="43"/>
       <c r="D46" s="53"/>
       <c r="E46" s="43"/>
       <c r="F46" s="43"/>
     </row>
-    <row r="47" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50"/>
       <c r="B47" s="52" t="s">
         <v>2</v>
@@ -3114,26 +3121,26 @@
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
     </row>
-    <row r="48" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E48" s="43"/>
       <c r="F48" s="46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E49" s="36">
         <v>11</v>
       </c>
       <c r="F49" s="53"/>
     </row>
-    <row r="50" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F50" s="53"/>
     </row>
-    <row r="51" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50"/>
       <c r="E51" s="43"/>
     </row>
-    <row r="52" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="50" t="s">
         <v>5</v>
       </c>
@@ -3142,15 +3149,15 @@
       </c>
       <c r="E52" s="43"/>
     </row>
-    <row r="53" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D53" s="42"/>
       <c r="E53" s="54"/>
     </row>
-    <row r="54" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D54" s="43"/>
       <c r="E54" s="54"/>
     </row>
-    <row r="55" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="50"/>
       <c r="B55" s="52" t="s">
         <v>3</v>
@@ -3161,14 +3168,14 @@
       <c r="D55" s="43"/>
       <c r="E55" s="54"/>
     </row>
-    <row r="56" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="42"/>
       <c r="D56" s="43"/>
       <c r="E56" s="46" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="43"/>
       <c r="D57" s="43">
         <v>10</v>
@@ -3176,29 +3183,29 @@
       <c r="H57" s="55"/>
       <c r="I57" s="55"/>
     </row>
-    <row r="58" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="43"/>
       <c r="D58" s="43"/>
     </row>
-    <row r="59" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="50"/>
       <c r="C59" s="43"/>
       <c r="D59" s="34" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="43">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="43"/>
     </row>
-    <row r="62" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="43"/>
     </row>
-    <row r="63" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="50"/>
       <c r="B63" s="52" t="s">
         <v>4</v>
@@ -3207,7 +3214,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" s="40"/>
       <c r="D64" s="40"/>
       <c r="E64" s="40"/>
@@ -3215,7 +3222,7 @@
       <c r="G64" s="40"/>
       <c r="H64" s="40"/>
     </row>
-    <row r="65" spans="1:8" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:8" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C65" s="40"/>
       <c r="D65" s="40"/>
       <c r="E65" s="40"/>
@@ -3223,7 +3230,7 @@
       <c r="G65" s="40"/>
       <c r="H65" s="40"/>
     </row>
-    <row r="66" spans="1:8" s="41" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" s="41" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
@@ -3232,7 +3239,7 @@
       <c r="G66" s="57"/>
       <c r="H66" s="40"/>
     </row>
-    <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="56"/>
       <c r="B67" s="66" t="s">
         <v>54</v>
@@ -3247,7 +3254,7 @@
       <c r="F67" s="63"/>
       <c r="H67" s="40"/>
     </row>
-    <row r="68" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" s="11"/>
       <c r="C68" s="68"/>
       <c r="D68" s="42"/>
@@ -3255,21 +3262,21 @@
       <c r="F68" s="63"/>
       <c r="H68" s="40"/>
     </row>
-    <row r="69" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
       <c r="D69" s="16"/>
       <c r="E69" s="64"/>
       <c r="F69" s="64"/>
     </row>
-    <row r="70" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
       <c r="D70" s="16"/>
       <c r="E70" s="64"/>
       <c r="F70" s="64"/>
     </row>
-    <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="16"/>
@@ -3280,28 +3287,28 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
       <c r="D72" s="62"/>
       <c r="E72" s="64"/>
       <c r="F72" s="64"/>
     </row>
-    <row r="73" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
       <c r="D73" s="16"/>
       <c r="E73" s="64"/>
       <c r="F73" s="64"/>
     </row>
-    <row r="74" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
       <c r="D74" s="16"/>
       <c r="E74" s="64"/>
       <c r="F74" s="64"/>
     </row>
-    <row r="75" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="11"/>
       <c r="C75" s="68" t="s">
         <v>61</v>
@@ -3312,41 +3319,41 @@
       <c r="E75" s="64"/>
       <c r="F75" s="64"/>
     </row>
-    <row r="76" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="11"/>
       <c r="C76" s="64"/>
       <c r="D76" s="64"/>
       <c r="E76" s="64"/>
       <c r="F76" s="64"/>
     </row>
-    <row r="77" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
     </row>
-    <row r="78" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
     </row>
-    <row r="79" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="65" t="s">
         <v>55</v>
       </c>
       <c r="F80" s="11"/>
     </row>
-    <row r="81" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B81" s="67" t="s">
         <v>58</v>
       </c>
@@ -3357,27 +3364,27 @@
       <c r="E81" s="63"/>
       <c r="F81" s="11"/>
     </row>
-    <row r="82" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C82" s="42"/>
       <c r="D82" s="63"/>
       <c r="E82" s="63"/>
       <c r="F82" s="11"/>
     </row>
-    <row r="83" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="11"/>
       <c r="C83" s="16"/>
       <c r="D83" s="64"/>
       <c r="E83" s="64"/>
       <c r="F83" s="11"/>
     </row>
-    <row r="84" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="11"/>
       <c r="C84" s="16"/>
       <c r="D84" s="64"/>
       <c r="E84" s="64"/>
       <c r="F84" s="11"/>
     </row>
-    <row r="85" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="11"/>
       <c r="C85" s="16"/>
       <c r="D85" s="7" t="s">
@@ -3388,28 +3395,28 @@
       </c>
       <c r="F85" s="11"/>
     </row>
-    <row r="86" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B86" s="11"/>
       <c r="C86" s="62"/>
       <c r="D86" s="64"/>
       <c r="E86" s="64"/>
       <c r="F86" s="11"/>
     </row>
-    <row r="87" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="11"/>
       <c r="C87" s="16"/>
       <c r="D87" s="64"/>
       <c r="E87" s="64"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="11"/>
       <c r="C88" s="16"/>
       <c r="D88" s="64"/>
       <c r="E88" s="64"/>
       <c r="F88" s="11"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89" s="68" t="s">
         <v>59</v>
       </c>
@@ -3420,7 +3427,7 @@
       <c r="E89" s="64"/>
       <c r="F89" s="11"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
@@ -3444,44 +3451,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10CBD3F-029F-4541-8142-F43EE81AFB98}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.36328125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="57" customWidth="1"/>
-    <col min="2" max="7" width="12.25" style="57" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="57" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="57" customWidth="1"/>
-    <col min="10" max="16384" width="17.375" style="57"/>
+    <col min="1" max="1" width="2.7265625" style="57" customWidth="1"/>
+    <col min="2" max="7" width="12.26953125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="57" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" style="57" customWidth="1"/>
+    <col min="10" max="16384" width="17.36328125" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="58"/>
       <c r="B1" s="40"/>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
       <c r="I1" s="40"/>
     </row>
-    <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
+    <row r="2" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
       <c r="I2" s="40"/>
     </row>
-    <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="79"/>
       <c r="B3" s="38" t="s">
         <v>26</v>
@@ -3494,43 +3501,43 @@
       <c r="H3" s="78"/>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:9" s="41" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="41" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="42"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="43"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="43">
         <v>1</v>
       </c>
       <c r="C8" s="42"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
       <c r="C9" s="43"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="43"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="43"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="44">
         <v>7</v>
       </c>
@@ -3538,68 +3545,68 @@
       <c r="E12" s="42"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="59"/>
       <c r="C13" s="43"/>
       <c r="E13" s="43"/>
     </row>
-    <row r="14" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
       <c r="E14" s="43"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="43"/>
       <c r="C15" s="34"/>
       <c r="E15" s="43"/>
       <c r="F15" s="19"/>
     </row>
-    <row r="16" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="43">
         <v>2</v>
       </c>
       <c r="E16" s="43"/>
       <c r="F16" s="19"/>
     </row>
-    <row r="17" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="35"/>
       <c r="E17" s="43"/>
       <c r="F17" s="19"/>
     </row>
-    <row r="18" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="43"/>
       <c r="F18" s="32"/>
       <c r="G18" s="76"/>
     </row>
-    <row r="19" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E19" s="43">
         <v>12</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="42"/>
     </row>
-    <row r="20" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E20" s="43"/>
       <c r="G20" s="43"/>
     </row>
-    <row r="21" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6"/>
       <c r="E21" s="43"/>
       <c r="G21" s="43"/>
     </row>
-    <row r="22" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="42"/>
       <c r="E22" s="43"/>
       <c r="G22" s="43"/>
     </row>
-    <row r="23" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="43"/>
       <c r="C23" s="6"/>
       <c r="E23" s="43"/>
       <c r="G23" s="43"/>
     </row>
-    <row r="24" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="43">
         <v>3</v>
       </c>
@@ -3608,20 +3615,20 @@
       <c r="G24" s="43"/>
       <c r="I24" s="47"/>
     </row>
-    <row r="25" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="35"/>
       <c r="C25" s="43"/>
       <c r="E25" s="43"/>
       <c r="G25" s="43"/>
       <c r="I25" s="43"/>
     </row>
-    <row r="26" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="43"/>
       <c r="E26" s="43"/>
       <c r="G26" s="43"/>
       <c r="I26" s="43"/>
     </row>
-    <row r="27" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="43"/>
       <c r="D27" s="33"/>
       <c r="E27" s="2"/>
@@ -3629,25 +3636,25 @@
       <c r="I27" s="43">
         <v>15</v>
       </c>
-      <c r="J27" s="88"/>
+      <c r="J27" s="82"/>
       <c r="K27" s="36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="43">
         <v>8</v>
       </c>
       <c r="G28" s="43"/>
       <c r="I28" s="43"/>
     </row>
-    <row r="29" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6"/>
       <c r="C29" s="43"/>
       <c r="G29" s="43"/>
       <c r="I29" s="35"/>
     </row>
-    <row r="30" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="42"/>
       <c r="C30" s="43"/>
       <c r="G30" s="43">
@@ -3655,18 +3662,18 @@
       </c>
       <c r="H30" s="45"/>
     </row>
-    <row r="31" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="43"/>
       <c r="C31" s="46"/>
       <c r="G31" s="43"/>
     </row>
-    <row r="32" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="43">
         <v>4</v>
       </c>
       <c r="G32" s="43"/>
     </row>
-    <row r="33" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="35"/>
       <c r="E33" s="50" t="s">
         <v>73</v>
@@ -3674,21 +3681,21 @@
       <c r="F33" s="6"/>
       <c r="G33" s="43"/>
     </row>
-    <row r="34" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F34" s="42"/>
       <c r="G34" s="43"/>
     </row>
-    <row r="35" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="84"/>
-      <c r="B35" s="84"/>
+    <row r="35" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="87"/>
+      <c r="B35" s="87"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
     </row>
-    <row r="36" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="87" t="s">
+    <row r="36" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="87"/>
+      <c r="B36" s="90"/>
       <c r="C36" s="50" t="s">
         <v>6</v>
       </c>
@@ -3696,17 +3703,17 @@
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
     </row>
-    <row r="37" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="43"/>
       <c r="F37" s="43"/>
       <c r="G37" s="43"/>
     </row>
-    <row r="38" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="43"/>
       <c r="F38" s="51"/>
       <c r="G38" s="43"/>
     </row>
-    <row r="39" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="50"/>
       <c r="B39" s="52" t="s">
         <v>1</v>
@@ -3715,14 +3722,14 @@
       <c r="F39" s="51"/>
       <c r="G39" s="43"/>
     </row>
-    <row r="40" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="42"/>
       <c r="D40" s="43"/>
       <c r="E40" s="33"/>
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
     </row>
-    <row r="41" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="43"/>
       <c r="D41" s="43">
         <v>9</v>
@@ -3731,7 +3738,7 @@
       <c r="F41" s="43"/>
       <c r="G41" s="46"/>
     </row>
-    <row r="42" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
       <c r="E42" s="43"/>
@@ -3739,14 +3746,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50"/>
       <c r="C43" s="43"/>
       <c r="D43" s="2"/>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
     </row>
-    <row r="44" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="43">
         <v>5</v>
       </c>
@@ -3754,18 +3761,18 @@
       <c r="E44" s="43"/>
       <c r="F44" s="43"/>
     </row>
-    <row r="45" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="43"/>
       <c r="E45" s="43"/>
       <c r="F45" s="43"/>
     </row>
-    <row r="46" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="43"/>
       <c r="D46" s="53"/>
       <c r="E46" s="43"/>
       <c r="F46" s="43"/>
     </row>
-    <row r="47" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="50"/>
       <c r="B47" s="52" t="s">
         <v>2</v>
@@ -3774,38 +3781,38 @@
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
     </row>
-    <row r="48" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E48" s="43"/>
       <c r="F48" s="46"/>
     </row>
-    <row r="49" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E49" s="36">
         <v>11</v>
       </c>
       <c r="F49" s="53"/>
     </row>
-    <row r="50" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F50" s="53"/>
     </row>
-    <row r="51" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50"/>
       <c r="E51" s="43"/>
     </row>
-    <row r="52" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="50" t="s">
         <v>5</v>
       </c>
       <c r="E52" s="43"/>
     </row>
-    <row r="53" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D53" s="42"/>
       <c r="E53" s="54"/>
     </row>
-    <row r="54" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D54" s="43"/>
       <c r="E54" s="54"/>
     </row>
-    <row r="55" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="50"/>
       <c r="B55" s="52" t="s">
         <v>3</v>
@@ -3813,12 +3820,12 @@
       <c r="D55" s="43"/>
       <c r="E55" s="54"/>
     </row>
-    <row r="56" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="42"/>
       <c r="D56" s="43"/>
       <c r="E56" s="46"/>
     </row>
-    <row r="57" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="43"/>
       <c r="D57" s="43">
         <v>10</v>
@@ -3826,34 +3833,34 @@
       <c r="H57" s="55"/>
       <c r="I57" s="55"/>
     </row>
-    <row r="58" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="43"/>
       <c r="D58" s="43"/>
     </row>
-    <row r="59" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="50"/>
       <c r="C59" s="43"/>
       <c r="D59" s="34"/>
     </row>
-    <row r="60" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="43">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="43"/>
     </row>
-    <row r="62" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="43"/>
     </row>
-    <row r="63" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="50"/>
       <c r="B63" s="52" t="s">
         <v>4</v>
       </c>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" s="40"/>
       <c r="D64" s="40"/>
       <c r="E64" s="40"/>
@@ -3861,7 +3868,7 @@
       <c r="G64" s="40"/>
       <c r="H64" s="40"/>
     </row>
-    <row r="65" spans="1:8" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:8" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C65" s="40"/>
       <c r="D65" s="40"/>
       <c r="E65" s="40"/>
@@ -3869,7 +3876,7 @@
       <c r="G65" s="40"/>
       <c r="H65" s="40"/>
     </row>
-    <row r="66" spans="1:8" s="41" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" s="41" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
@@ -3878,7 +3885,7 @@
       <c r="G66" s="57"/>
       <c r="H66" s="40"/>
     </row>
-    <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="56"/>
       <c r="B67" s="66" t="s">
         <v>54</v>
@@ -3891,7 +3898,7 @@
       <c r="F67" s="63"/>
       <c r="H67" s="40"/>
     </row>
-    <row r="68" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" s="11"/>
       <c r="C68" s="68"/>
       <c r="D68" s="42"/>
@@ -3899,21 +3906,21 @@
       <c r="F68" s="63"/>
       <c r="H68" s="40"/>
     </row>
-    <row r="69" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
       <c r="D69" s="16"/>
       <c r="E69" s="64"/>
       <c r="F69" s="64"/>
     </row>
-    <row r="70" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
       <c r="D70" s="16"/>
       <c r="E70" s="64"/>
       <c r="F70" s="64"/>
     </row>
-    <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="16"/>
@@ -3922,28 +3929,28 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
       <c r="D72" s="62"/>
       <c r="E72" s="64"/>
       <c r="F72" s="64"/>
     </row>
-    <row r="73" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
       <c r="D73" s="16"/>
       <c r="E73" s="64"/>
       <c r="F73" s="64"/>
     </row>
-    <row r="74" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
       <c r="D74" s="16"/>
       <c r="E74" s="64"/>
       <c r="F74" s="64"/>
     </row>
-    <row r="75" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="11"/>
       <c r="C75" s="68" t="s">
         <v>61</v>
@@ -3952,41 +3959,41 @@
       <c r="E75" s="64"/>
       <c r="F75" s="64"/>
     </row>
-    <row r="76" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="11"/>
       <c r="C76" s="64"/>
       <c r="D76" s="64"/>
       <c r="E76" s="64"/>
       <c r="F76" s="64"/>
     </row>
-    <row r="77" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
     </row>
-    <row r="78" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
     </row>
-    <row r="79" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="65" t="s">
         <v>55</v>
       </c>
       <c r="F80" s="11"/>
     </row>
-    <row r="81" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B81" s="67" t="s">
         <v>58</v>
       </c>
@@ -3995,27 +4002,27 @@
       <c r="E81" s="63"/>
       <c r="F81" s="11"/>
     </row>
-    <row r="82" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C82" s="42"/>
       <c r="D82" s="63"/>
       <c r="E82" s="63"/>
       <c r="F82" s="11"/>
     </row>
-    <row r="83" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="11"/>
       <c r="C83" s="16"/>
       <c r="D83" s="64"/>
       <c r="E83" s="64"/>
       <c r="F83" s="11"/>
     </row>
-    <row r="84" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="11"/>
       <c r="C84" s="16"/>
       <c r="D84" s="64"/>
       <c r="E84" s="64"/>
       <c r="F84" s="11"/>
     </row>
-    <row r="85" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="11"/>
       <c r="C85" s="16"/>
       <c r="D85" s="7" t="s">
@@ -4026,28 +4033,28 @@
       </c>
       <c r="F85" s="11"/>
     </row>
-    <row r="86" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B86" s="11"/>
       <c r="C86" s="62"/>
       <c r="D86" s="64"/>
       <c r="E86" s="64"/>
       <c r="F86" s="11"/>
     </row>
-    <row r="87" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="11"/>
       <c r="C87" s="16"/>
       <c r="D87" s="64"/>
       <c r="E87" s="64"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="2:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="11"/>
       <c r="C88" s="16"/>
       <c r="D88" s="64"/>
       <c r="E88" s="64"/>
       <c r="F88" s="11"/>
     </row>
-    <row r="89" spans="2:6" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89" s="68" t="s">
         <v>59</v>
       </c>
@@ -4056,7 +4063,7 @@
       <c r="E89" s="64"/>
       <c r="F89" s="11"/>
     </row>
-    <row r="90" spans="2:6" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
@@ -4073,4 +4080,640 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDD3758-D1D3-4DDF-ADF0-FED2CD00CB37}">
+  <dimension ref="A1:K90"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.36328125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.7265625" style="57" customWidth="1"/>
+    <col min="2" max="7" width="12.26953125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="57" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" style="57" customWidth="1"/>
+    <col min="10" max="16384" width="17.36328125" style="57"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="58"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="40"/>
+    </row>
+    <row r="2" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="40"/>
+    </row>
+    <row r="3" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="81"/>
+      <c r="B3" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="40"/>
+    </row>
+    <row r="4" spans="1:9" s="41" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="42"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="43"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="43">
+        <v>1</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="2"/>
+      <c r="C9" s="43"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="43"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="43"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="44">
+        <v>7</v>
+      </c>
+      <c r="D12" s="45"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="59"/>
+      <c r="C13" s="43"/>
+      <c r="E13" s="43"/>
+    </row>
+    <row r="14" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="43"/>
+      <c r="C15" s="34"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="43">
+        <v>2</v>
+      </c>
+      <c r="E16" s="43"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="35"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="43"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="76"/>
+    </row>
+    <row r="19" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="43">
+        <v>12</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="42"/>
+    </row>
+    <row r="20" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="43"/>
+      <c r="G20" s="43"/>
+    </row>
+    <row r="21" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="6"/>
+      <c r="E21" s="43"/>
+      <c r="G21" s="43"/>
+    </row>
+    <row r="22" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="G22" s="43"/>
+    </row>
+    <row r="23" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="43"/>
+      <c r="C23" s="6"/>
+      <c r="E23" s="43"/>
+      <c r="G23" s="43"/>
+    </row>
+    <row r="24" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="43">
+        <v>3</v>
+      </c>
+      <c r="C24" s="48"/>
+      <c r="E24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="I24" s="47"/>
+    </row>
+    <row r="25" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="35"/>
+      <c r="C25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="I25" s="43"/>
+    </row>
+    <row r="26" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="43"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="2"/>
+      <c r="G27" s="43"/>
+      <c r="I27" s="43">
+        <v>15</v>
+      </c>
+      <c r="J27" s="82"/>
+      <c r="K27" s="36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="43">
+        <v>8</v>
+      </c>
+      <c r="G28" s="43"/>
+      <c r="I28" s="43"/>
+    </row>
+    <row r="29" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6"/>
+      <c r="C29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="I29" s="35"/>
+    </row>
+    <row r="30" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="G30" s="43">
+        <v>14</v>
+      </c>
+      <c r="H30" s="45"/>
+    </row>
+    <row r="31" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="43"/>
+      <c r="C31" s="46"/>
+      <c r="G31" s="43"/>
+    </row>
+    <row r="32" spans="2:11" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="43">
+        <v>4</v>
+      </c>
+      <c r="G32" s="43"/>
+    </row>
+    <row r="33" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="35"/>
+      <c r="E33" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="43"/>
+    </row>
+    <row r="34" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="42"/>
+      <c r="G34" s="43"/>
+    </row>
+    <row r="35" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="87"/>
+      <c r="B35" s="87"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+    </row>
+    <row r="36" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="90"/>
+      <c r="C36" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="47"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+    </row>
+    <row r="37" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+    </row>
+    <row r="38" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="43"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="43"/>
+    </row>
+    <row r="39" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="50"/>
+      <c r="B39" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="43"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="43"/>
+    </row>
+    <row r="40" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="42"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+    </row>
+    <row r="41" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="43"/>
+      <c r="D41" s="43">
+        <v>9</v>
+      </c>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="46"/>
+    </row>
+    <row r="42" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="50"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+    </row>
+    <row r="44" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="43">
+        <v>5</v>
+      </c>
+      <c r="D44" s="45"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+    </row>
+    <row r="45" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+    </row>
+    <row r="46" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="43"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+    </row>
+    <row r="47" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="50"/>
+      <c r="B47" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+    </row>
+    <row r="48" spans="1:7" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="43"/>
+      <c r="F48" s="46"/>
+    </row>
+    <row r="49" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E49" s="36">
+        <v>11</v>
+      </c>
+      <c r="F49" s="53"/>
+    </row>
+    <row r="50" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="53"/>
+    </row>
+    <row r="51" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="50"/>
+      <c r="E51" s="43"/>
+    </row>
+    <row r="52" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="43"/>
+    </row>
+    <row r="53" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="42"/>
+      <c r="E53" s="54"/>
+    </row>
+    <row r="54" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="43"/>
+      <c r="E54" s="54"/>
+    </row>
+    <row r="55" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="50"/>
+      <c r="B55" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="43"/>
+      <c r="E55" s="54"/>
+    </row>
+    <row r="56" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="42"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="46"/>
+    </row>
+    <row r="57" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="43"/>
+      <c r="D57" s="43">
+        <v>10</v>
+      </c>
+      <c r="H57" s="55"/>
+      <c r="I57" s="55"/>
+    </row>
+    <row r="58" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+    </row>
+    <row r="59" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="50"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="34"/>
+    </row>
+    <row r="60" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="43"/>
+    </row>
+    <row r="62" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="43"/>
+    </row>
+    <row r="63" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="50"/>
+      <c r="B63" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:9" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="40"/>
+      <c r="H64" s="40"/>
+    </row>
+    <row r="65" spans="1:8" s="36" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+    </row>
+    <row r="66" spans="1:8" s="41" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="57"/>
+      <c r="H66" s="40"/>
+    </row>
+    <row r="67" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="56"/>
+      <c r="B67" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="D67" s="72"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="H67" s="40"/>
+    </row>
+    <row r="68" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" s="11"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="63"/>
+      <c r="H68" s="40"/>
+    </row>
+    <row r="69" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+    </row>
+    <row r="70" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="64"/>
+      <c r="F70" s="64"/>
+    </row>
+    <row r="71" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="77"/>
+      <c r="F71" s="64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="62"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+    </row>
+    <row r="73" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+    </row>
+    <row r="74" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+    </row>
+    <row r="75" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="11"/>
+      <c r="C75" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="D75" s="5"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+    </row>
+    <row r="76" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="11"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+    </row>
+    <row r="77" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+    </row>
+    <row r="78" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+    </row>
+    <row r="79" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+    </row>
+    <row r="80" spans="1:8" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B80" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="F80" s="11"/>
+    </row>
+    <row r="81" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="C81" s="47"/>
+      <c r="D81" s="63"/>
+      <c r="E81" s="63"/>
+      <c r="F81" s="11"/>
+    </row>
+    <row r="82" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C82" s="42"/>
+      <c r="D82" s="63"/>
+      <c r="E82" s="63"/>
+      <c r="F82" s="11"/>
+    </row>
+    <row r="83" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="11"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B84" s="11"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
+      <c r="F84" s="11"/>
+    </row>
+    <row r="85" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B85" s="11"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E85" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="F85" s="11"/>
+    </row>
+    <row r="86" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="11"/>
+      <c r="C86" s="62"/>
+      <c r="D86" s="64"/>
+      <c r="E86" s="64"/>
+      <c r="F86" s="11"/>
+    </row>
+    <row r="87" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="11"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="64"/>
+      <c r="E87" s="64"/>
+      <c r="F87" s="11"/>
+    </row>
+    <row r="88" spans="2:6" ht="11.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="11"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="64"/>
+      <c r="E88" s="64"/>
+      <c r="F88" s="11"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B89" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="64"/>
+      <c r="E89" s="64"/>
+      <c r="F89" s="11"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 4th tournament
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C91916-3B58-4326-8153-C9F310D233A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AEB11B-04DE-47F2-87A7-8C557429B954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="115">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -452,6 +452,26 @@
   </si>
   <si>
     <t>金贝贝(6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">钱夫人(3) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忍太郎(2)   1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莎拉公主(8)   3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰乔(1)   3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孙小美(7)   0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -828,6 +848,17 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -852,17 +883,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1219,25 +1239,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -1468,17 +1488,17 @@
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="84"/>
-      <c r="B35" s="84"/>
+      <c r="A35" s="89"/>
+      <c r="B35" s="89"/>
       <c r="C35" s="22"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="82"/>
+      <c r="B36" s="87"/>
       <c r="C36" s="21" t="s">
         <v>6</v>
       </c>
@@ -1674,45 +1694,45 @@
       </c>
     </row>
     <row r="64" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="81"/>
-      <c r="D64" s="81"/>
-      <c r="E64" s="81"/>
-      <c r="F64" s="81"/>
-      <c r="G64" s="81"/>
-      <c r="H64" s="81"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="86"/>
+      <c r="G64" s="86"/>
+      <c r="H64" s="86"/>
     </row>
     <row r="65" spans="1:8" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="81"/>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
-      <c r="F65" s="81"/>
-      <c r="G65" s="81"/>
-      <c r="H65" s="81"/>
+      <c r="C65" s="86"/>
+      <c r="D65" s="86"/>
+      <c r="E65" s="86"/>
+      <c r="F65" s="86"/>
+      <c r="G65" s="86"/>
+      <c r="H65" s="86"/>
     </row>
     <row r="66" spans="1:8" s="12" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="81"/>
-      <c r="D66" s="81"/>
-      <c r="E66" s="81"/>
-      <c r="F66" s="81"/>
-      <c r="G66" s="81"/>
-      <c r="H66" s="81"/>
+      <c r="C66" s="86"/>
+      <c r="D66" s="86"/>
+      <c r="E66" s="86"/>
+      <c r="F66" s="86"/>
+      <c r="G66" s="86"/>
+      <c r="H66" s="86"/>
     </row>
     <row r="67" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="28"/>
-      <c r="C67" s="81"/>
-      <c r="D67" s="81"/>
-      <c r="E67" s="81"/>
-      <c r="F67" s="81"/>
-      <c r="G67" s="81"/>
-      <c r="H67" s="81"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="86"/>
+      <c r="E67" s="86"/>
+      <c r="F67" s="86"/>
+      <c r="G67" s="86"/>
+      <c r="H67" s="86"/>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C68" s="81"/>
-      <c r="D68" s="81"/>
-      <c r="E68" s="81"/>
-      <c r="F68" s="81"/>
-      <c r="G68" s="81"/>
-      <c r="H68" s="81"/>
+      <c r="C68" s="86"/>
+      <c r="D68" s="86"/>
+      <c r="E68" s="86"/>
+      <c r="F68" s="86"/>
+      <c r="G68" s="86"/>
+      <c r="H68" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1748,25 +1768,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -2182,8 +2202,8 @@
       <c r="I34" s="36"/>
     </row>
     <row r="35" spans="1:9" s="4" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="85"/>
-      <c r="B35" s="85"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="90"/>
       <c r="C35" s="36"/>
       <c r="D35" s="36"/>
       <c r="E35" s="36"/>
@@ -2781,25 +2801,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="58"/>
       <c r="B1" s="40"/>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
       <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
       <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -3042,16 +3062,16 @@
       <c r="G34" s="43"/>
     </row>
     <row r="35" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="85"/>
-      <c r="B35" s="85"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="90"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
     </row>
     <row r="36" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="88"/>
+      <c r="B36" s="93"/>
       <c r="C36" s="50" t="s">
         <v>6</v>
       </c>
@@ -3480,8 +3500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10CBD3F-029F-4541-8142-F43EE81AFB98}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -3496,25 +3516,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="58"/>
       <c r="B1" s="40"/>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
       <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
       <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -3536,7 +3556,7 @@
     </row>
     <row r="5" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="36" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -3547,6 +3567,9 @@
     </row>
     <row r="7" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="43"/>
+      <c r="C7" s="36" t="s">
+        <v>104</v>
+      </c>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -3557,8 +3580,8 @@
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35" t="s">
-        <v>104</v>
+      <c r="B9" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="C9" s="43"/>
       <c r="F9" s="14"/>
@@ -3580,8 +3603,8 @@
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="89" t="s">
-        <v>105</v>
+      <c r="B13" s="81" t="s">
+        <v>111</v>
       </c>
       <c r="C13" s="43"/>
       <c r="E13" s="43"/>
@@ -3594,7 +3617,9 @@
     </row>
     <row r="15" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="43"/>
-      <c r="C15" s="46"/>
+      <c r="C15" s="46" t="s">
+        <v>106</v>
+      </c>
       <c r="E15" s="43"/>
       <c r="F15" s="19"/>
     </row>
@@ -3606,8 +3631,8 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="35" t="s">
-        <v>106</v>
+      <c r="B17" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="19"/>
@@ -3629,8 +3654,8 @@
       <c r="G20" s="43"/>
     </row>
     <row r="21" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="36" t="s">
-        <v>107</v>
+      <c r="B21" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="E21" s="43"/>
       <c r="G21" s="43"/>
@@ -3642,6 +3667,9 @@
     </row>
     <row r="23" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="43"/>
+      <c r="C23" s="36" t="s">
+        <v>107</v>
+      </c>
       <c r="E23" s="43"/>
       <c r="G23" s="43"/>
     </row>
@@ -3656,7 +3684,7 @@
     </row>
     <row r="25" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="35" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C25" s="43"/>
       <c r="E25" s="43"/>
@@ -3677,7 +3705,7 @@
       <c r="I27" s="43">
         <v>15</v>
       </c>
-      <c r="J27" s="90"/>
+      <c r="J27" s="82"/>
       <c r="K27" s="36" t="s">
         <v>40</v>
       </c>
@@ -3730,16 +3758,16 @@
       <c r="G34" s="43"/>
     </row>
     <row r="35" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="85"/>
-      <c r="B35" s="85"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="90"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
     </row>
     <row r="36" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="88"/>
+      <c r="B36" s="93"/>
       <c r="C36" s="50" t="s">
         <v>6</v>
       </c>
@@ -3761,6 +3789,9 @@
       <c r="A39" s="50"/>
       <c r="B39" s="52" t="s">
         <v>1</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>110</v>
       </c>
       <c r="D39" s="43"/>
       <c r="F39" s="51"/>
@@ -3821,7 +3852,9 @@
       <c r="B47" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="35"/>
+      <c r="C47" s="35" t="s">
+        <v>105</v>
+      </c>
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
     </row>
@@ -3860,6 +3893,9 @@
       <c r="A55" s="50"/>
       <c r="B55" s="52" t="s">
         <v>3</v>
+      </c>
+      <c r="C55" s="36" t="s">
+        <v>108</v>
       </c>
       <c r="D55" s="43"/>
       <c r="E55" s="54"/>
@@ -3934,7 +3970,7 @@
       <c r="B67" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="C67" s="91" t="s">
+      <c r="C67" s="83" t="s">
         <v>60</v>
       </c>
       <c r="D67" s="70"/>
@@ -3961,13 +3997,13 @@
     </row>
     <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D71" s="43"/>
-      <c r="E71" s="92"/>
+      <c r="E71" s="84"/>
       <c r="F71" s="63" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="93"/>
+      <c r="D72" s="85"/>
       <c r="E72" s="63"/>
       <c r="F72" s="63"/>
     </row>
@@ -4034,7 +4070,7 @@
       </c>
     </row>
     <row r="86" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C86" s="93"/>
+      <c r="C86" s="85"/>
       <c r="D86" s="63"/>
       <c r="E86" s="63"/>
     </row>
@@ -4088,25 +4124,25 @@
     <row r="1" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="58"/>
       <c r="B1" s="40"/>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
       <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
       <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.4">
@@ -4167,7 +4203,7 @@
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="89"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="43"/>
       <c r="E13" s="43"/>
     </row>
@@ -4255,7 +4291,7 @@
       <c r="I27" s="43">
         <v>15</v>
       </c>
-      <c r="J27" s="90"/>
+      <c r="J27" s="82"/>
       <c r="K27" s="36" t="s">
         <v>40</v>
       </c>
@@ -4303,16 +4339,16 @@
       <c r="G34" s="43"/>
     </row>
     <row r="35" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="85"/>
-      <c r="B35" s="85"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="90"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
     </row>
     <row r="36" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="88"/>
+      <c r="B36" s="93"/>
       <c r="C36" s="50" t="s">
         <v>6</v>
       </c>
@@ -4507,7 +4543,7 @@
       <c r="B67" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="C67" s="91" t="s">
+      <c r="C67" s="83" t="s">
         <v>60</v>
       </c>
       <c r="D67" s="70"/>
@@ -4534,13 +4570,13 @@
     </row>
     <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D71" s="43"/>
-      <c r="E71" s="92"/>
+      <c r="E71" s="84"/>
       <c r="F71" s="63" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="93"/>
+      <c r="D72" s="85"/>
       <c r="E72" s="63"/>
       <c r="F72" s="63"/>
     </row>
@@ -4607,7 +4643,7 @@
       </c>
     </row>
     <row r="86" spans="2:5" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C86" s="93"/>
+      <c r="C86" s="85"/>
       <c r="D86" s="63"/>
       <c r="E86" s="63"/>
     </row>

</xml_diff>

<commit_message>
Update on 5th Match
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AEB11B-04DE-47F2-87A7-8C557429B954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66688FCD-149A-4F2F-B3BC-A82EC94D8BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="119">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -472,6 +472,22 @@
   </si>
   <si>
     <t>孙小美(7)   0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙隆巴斯(4)   2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金贝贝(6)   3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钱夫人(3)    3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忍太郎(2)   2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3500,8 +3516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10CBD3F-029F-4541-8142-F43EE81AFB98}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -3719,7 +3735,7 @@
     </row>
     <row r="29" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="C29" s="43"/>
       <c r="G29" s="43"/>
@@ -3735,7 +3751,9 @@
     </row>
     <row r="31" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="43"/>
-      <c r="C31" s="46"/>
+      <c r="C31" s="46" t="s">
+        <v>109</v>
+      </c>
       <c r="G31" s="43"/>
     </row>
     <row r="32" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -3745,8 +3763,8 @@
       <c r="G32" s="43"/>
     </row>
     <row r="33" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="35" t="s">
-        <v>109</v>
+      <c r="B33" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="E33" s="50" t="s">
         <v>73</v>
@@ -3790,8 +3808,8 @@
       <c r="B39" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="36" t="s">
-        <v>110</v>
+      <c r="C39" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="D39" s="43"/>
       <c r="F39" s="51"/>
@@ -3824,7 +3842,9 @@
     <row r="43" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50"/>
       <c r="C43" s="43"/>
-      <c r="D43" s="35"/>
+      <c r="D43" s="35" t="s">
+        <v>110</v>
+      </c>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
     </row>
@@ -3853,7 +3873,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
@@ -3938,7 +3958,9 @@
       <c r="B63" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C63" s="35"/>
+      <c r="C63" s="35" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="64" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C64" s="40"/>
@@ -4043,7 +4065,9 @@
       <c r="B81" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="C81" s="47"/>
+      <c r="C81" s="47" t="s">
+        <v>105</v>
+      </c>
       <c r="D81" s="63"/>
       <c r="E81" s="63"/>
     </row>

</xml_diff>

<commit_message>
5-6th place match updated
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lts\Documents\GitHub\2018_world_cup_draw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36953618-34C8-4BF4-A6E2-046618C6F96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9911626D-C02A-4659-A294-67507AD2C2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="123">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -448,10 +448,6 @@
   </si>
   <si>
     <t>孙小美(7)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>金贝贝(6)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3536,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10CBD3F-029F-4541-8142-F43EE81AFB98}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -3643,7 +3639,7 @@
     </row>
     <row r="13" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" s="43"/>
       <c r="E13" s="43"/>
@@ -3657,7 +3653,7 @@
     <row r="15" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="43"/>
       <c r="C15" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E15" s="43"/>
       <c r="F15" s="19"/>
@@ -3671,7 +3667,7 @@
     </row>
     <row r="17" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="19"/>
@@ -3694,7 +3690,7 @@
     </row>
     <row r="21" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21" s="43"/>
       <c r="G21" s="43"/>
@@ -3707,7 +3703,7 @@
     <row r="23" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="43"/>
       <c r="C23" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E23" s="43"/>
       <c r="G23" s="43"/>
@@ -3723,7 +3719,7 @@
     </row>
     <row r="25" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="43"/>
       <c r="E25" s="43"/>
@@ -3760,7 +3756,7 @@
     </row>
     <row r="29" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" s="43"/>
       <c r="G29" s="43"/>
@@ -3777,7 +3773,7 @@
     <row r="31" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="43"/>
       <c r="C31" s="46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G31" s="43"/>
     </row>
@@ -3789,7 +3785,7 @@
     </row>
     <row r="33" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="50" t="s">
         <v>73</v>
@@ -3815,7 +3811,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
@@ -3836,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D39" s="43"/>
       <c r="F39" s="51"/>
@@ -3846,7 +3842,7 @@
       <c r="C40" s="42"/>
       <c r="D40" s="43"/>
       <c r="E40" s="49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
@@ -3872,7 +3868,7 @@
       <c r="A43" s="50"/>
       <c r="C43" s="43"/>
       <c r="D43" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
@@ -3902,7 +3898,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
@@ -3947,7 +3943,7 @@
         <v>3</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D55" s="43"/>
       <c r="E55" s="54"/>
@@ -3975,7 +3971,7 @@
       <c r="A59" s="50"/>
       <c r="C59" s="43"/>
       <c r="D59" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -3995,7 +3991,7 @@
         <v>4</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
@@ -4032,7 +4028,7 @@
         <v>60</v>
       </c>
       <c r="D67" s="70" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="E67" s="63"/>
       <c r="F67" s="63"/>
@@ -4057,7 +4053,9 @@
     </row>
     <row r="71" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D71" s="43"/>
-      <c r="E71" s="84"/>
+      <c r="E71" s="84" t="s">
+        <v>104</v>
+      </c>
       <c r="F71" s="63" t="s">
         <v>56</v>
       </c>
@@ -4081,8 +4079,8 @@
       <c r="C75" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="D75" s="35" t="s">
-        <v>104</v>
+      <c r="D75" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="E75" s="63"/>
       <c r="F75" s="63"/>
@@ -4106,7 +4104,7 @@
         <v>58</v>
       </c>
       <c r="C81" s="76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D81" s="63"/>
       <c r="E81" s="63"/>
@@ -4155,7 +4153,7 @@
         <v>59</v>
       </c>
       <c r="C89" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D89" s="63"/>
       <c r="E89" s="63"/>

</xml_diff>

<commit_message>
Final Match 1 Updated
</commit_message>
<xml_diff>
--- a/8-team-double.xlsx
+++ b/8-team-double.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\GitHub\2018_world_cup_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF76B374-0F0E-4962-8BD7-BED8B7CAB342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E84ED1-80B1-4635-B743-5326C165B48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="126">
   <si>
     <t>PrintYourBrackets</t>
   </si>
@@ -439,10 +439,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>莎拉公主(8)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>约翰乔(1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -508,6 +504,18 @@
   </si>
   <si>
     <t>莎拉公主(8)   0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莎拉公主(8)   1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰乔(1)   1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Match 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3537,7 +3545,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -3629,7 +3637,7 @@
     <row r="11" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="43"/>
       <c r="E11" s="36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" s="14"/>
     </row>
@@ -3643,7 +3651,7 @@
     </row>
     <row r="13" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="81" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="43"/>
       <c r="E13" s="43"/>
@@ -3657,7 +3665,7 @@
     <row r="15" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="43"/>
       <c r="C15" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" s="43"/>
       <c r="F15" s="19"/>
@@ -3671,7 +3679,7 @@
     </row>
     <row r="17" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="19"/>
@@ -3680,7 +3688,7 @@
       <c r="E18" s="43"/>
       <c r="F18" s="32"/>
       <c r="G18" s="47" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -3696,7 +3704,7 @@
     </row>
     <row r="21" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E21" s="43"/>
       <c r="G21" s="43"/>
@@ -3709,7 +3717,7 @@
     <row r="23" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="43"/>
       <c r="C23" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E23" s="43"/>
       <c r="G23" s="43"/>
@@ -3721,11 +3729,16 @@
       <c r="C24" s="48"/>
       <c r="E24" s="43"/>
       <c r="G24" s="43"/>
-      <c r="I24" s="47"/>
+      <c r="H24" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" s="47" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="25" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" s="43"/>
       <c r="E25" s="43"/>
@@ -3742,7 +3755,7 @@
       <c r="C27" s="43"/>
       <c r="D27" s="49"/>
       <c r="E27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G27" s="43"/>
       <c r="I27" s="43">
@@ -3762,11 +3775,13 @@
     </row>
     <row r="29" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" s="43"/>
       <c r="G29" s="43"/>
-      <c r="I29" s="35"/>
+      <c r="I29" s="35" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="30" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="42"/>
@@ -3779,7 +3794,7 @@
     <row r="31" spans="2:11" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="43"/>
       <c r="C31" s="46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G31" s="43"/>
     </row>
@@ -3791,13 +3806,13 @@
     </row>
     <row r="33" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E33" s="50" t="s">
         <v>73</v>
       </c>
       <c r="F33" s="36" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="G33" s="43"/>
     </row>
@@ -3820,7 +3835,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
@@ -3841,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D39" s="43"/>
       <c r="F39" s="51"/>
@@ -3851,7 +3866,7 @@
       <c r="C40" s="42"/>
       <c r="D40" s="43"/>
       <c r="E40" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
@@ -3863,7 +3878,9 @@
       </c>
       <c r="E41" s="43"/>
       <c r="F41" s="43"/>
-      <c r="G41" s="46"/>
+      <c r="G41" s="34" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="42" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="43"/>
@@ -3877,7 +3894,7 @@
       <c r="A43" s="50"/>
       <c r="C43" s="43"/>
       <c r="D43" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
@@ -3907,15 +3924,15 @@
         <v>2</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
     </row>
     <row r="48" spans="1:7" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E48" s="43"/>
-      <c r="F48" s="46" t="s">
-        <v>108</v>
+      <c r="F48" s="34" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -3954,7 +3971,7 @@
         <v>3</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D55" s="43"/>
       <c r="E55" s="54"/>
@@ -3963,7 +3980,7 @@
       <c r="C56" s="42"/>
       <c r="D56" s="43"/>
       <c r="E56" s="46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -3982,7 +3999,7 @@
       <c r="A59" s="50"/>
       <c r="C59" s="43"/>
       <c r="D59" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.3">
@@ -4002,7 +4019,7 @@
         <v>4</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="36" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.4">
@@ -4039,7 +4056,7 @@
         <v>60</v>
       </c>
       <c r="D67" s="70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E67" s="63"/>
       <c r="F67" s="63"/>
@@ -4115,7 +4132,7 @@
         <v>58</v>
       </c>
       <c r="C81" s="76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D81" s="63"/>
       <c r="E81" s="63"/>
@@ -4164,7 +4181,7 @@
         <v>59</v>
       </c>
       <c r="C89" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D89" s="63"/>
       <c r="E89" s="63"/>

</xml_diff>